<commit_message>
Fixed one typo and rebuilt templates with updated transformation intensities
</commit_message>
<xml_diff>
--- a/iran/transformations/templates/calibrated/iran/model_input_variables_iran_ce_calibrated.xlsx
+++ b/iran/transformations/templates/calibrated/iran/model_input_variables_iran_ce_calibrated.xlsx
@@ -29046,76 +29046,76 @@
         <v>0.0024171763506625</v>
       </c>
       <c r="V2">
-        <v>0.002360456543003326</v>
+        <v>0.002404452416621757</v>
       </c>
       <c r="W2">
-        <v>0.002303736735344153</v>
+        <v>0.002391728482581014</v>
       </c>
       <c r="X2">
-        <v>0.002247016927684979</v>
+        <v>0.002379004548540271</v>
       </c>
       <c r="Y2">
-        <v>0.002190297120025806</v>
+        <v>0.002366280614499528</v>
       </c>
       <c r="Z2">
-        <v>0.002133577312366632</v>
+        <v>0.002353556680458785</v>
       </c>
       <c r="AA2">
-        <v>0.002076857504707458</v>
+        <v>0.002340832746418041</v>
       </c>
       <c r="AB2">
-        <v>0.002020137697048285</v>
+        <v>0.002328108812377298</v>
       </c>
       <c r="AC2">
-        <v>0.001963417889389111</v>
+        <v>0.002315384878336556</v>
       </c>
       <c r="AD2">
-        <v>0.001906698081729937</v>
+        <v>0.002302660944295812</v>
       </c>
       <c r="AE2">
-        <v>0.001849978274070764</v>
+        <v>0.002289937010255069</v>
       </c>
       <c r="AF2">
-        <v>0.00179325846641159</v>
+        <v>0.002277213076214326</v>
       </c>
       <c r="AG2">
-        <v>0.001736538658752416</v>
+        <v>0.002264489142173583</v>
       </c>
       <c r="AH2">
-        <v>0.001679818851093243</v>
+        <v>0.00225176520813284</v>
       </c>
       <c r="AI2">
-        <v>0.001623099043434069</v>
+        <v>0.002239041274092097</v>
       </c>
       <c r="AJ2">
-        <v>0.001566379235774896</v>
+        <v>0.002226317340051354</v>
       </c>
       <c r="AK2">
-        <v>0.001509659428115722</v>
+        <v>0.002213593406010611</v>
       </c>
       <c r="AL2">
-        <v>0.001452939620456548</v>
+        <v>0.002200869471969868</v>
       </c>
       <c r="AM2">
-        <v>0.001396219812797375</v>
+        <v>0.002188145537929125</v>
       </c>
       <c r="AN2">
-        <v>0.001339500005138201</v>
+        <v>0.002175421603888381</v>
       </c>
       <c r="AO2">
-        <v>0.001282780197479027</v>
+        <v>0.002162697669847638</v>
       </c>
       <c r="AP2">
-        <v>0.001226060389819854</v>
+        <v>0.002149973735806895</v>
       </c>
       <c r="AQ2">
-        <v>0.00116934058216068</v>
+        <v>0.002137249801766152</v>
       </c>
       <c r="AR2">
-        <v>0.001112620774501507</v>
+        <v>0.002124525867725409</v>
       </c>
       <c r="AS2">
-        <v>0.001055900966842333</v>
+        <v>0.002111801933684666</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -29171,76 +29171,76 @@
         <v>0.7710792558613661</v>
       </c>
       <c r="V3">
-        <v>0.7764509535338091</v>
+        <v>0.7722842868671425</v>
       </c>
       <c r="W3">
-        <v>0.7818226512062522</v>
+        <v>0.7734893178729189</v>
       </c>
       <c r="X3">
-        <v>0.7871943488786953</v>
+        <v>0.7746943488786953</v>
       </c>
       <c r="Y3">
-        <v>0.7925660465511384</v>
+        <v>0.7758993798844717</v>
       </c>
       <c r="Z3">
-        <v>0.7979377442235814</v>
+        <v>0.7771044108902481</v>
       </c>
       <c r="AA3">
-        <v>0.8033094418960245</v>
+        <v>0.7783094418960246</v>
       </c>
       <c r="AB3">
-        <v>0.8086811395684677</v>
+        <v>0.779514472901801</v>
       </c>
       <c r="AC3">
-        <v>0.8140528372409108</v>
+        <v>0.7807195039075774</v>
       </c>
       <c r="AD3">
-        <v>0.8194245349133538</v>
+        <v>0.7819245349133539</v>
       </c>
       <c r="AE3">
-        <v>0.8247962325857968</v>
+        <v>0.7831295659191302</v>
       </c>
       <c r="AF3">
-        <v>0.83016793025824</v>
+        <v>0.7843345969249067</v>
       </c>
       <c r="AG3">
-        <v>0.835539627930683</v>
+        <v>0.785539627930683</v>
       </c>
       <c r="AH3">
-        <v>0.8409113256031262</v>
+        <v>0.7867446589364595</v>
       </c>
       <c r="AI3">
-        <v>0.8462830232755691</v>
+        <v>0.7879496899422359</v>
       </c>
       <c r="AJ3">
-        <v>0.8516547209480123</v>
+        <v>0.7891547209480123</v>
       </c>
       <c r="AK3">
-        <v>0.8570264186204554</v>
+        <v>0.7903597519537887</v>
       </c>
       <c r="AL3">
-        <v>0.8623981162928984</v>
+        <v>0.7915647829595651</v>
       </c>
       <c r="AM3">
-        <v>0.8677698139653416</v>
+        <v>0.7927698139653416</v>
       </c>
       <c r="AN3">
-        <v>0.8731415116377846</v>
+        <v>0.7939748449711179</v>
       </c>
       <c r="AO3">
-        <v>0.8785132093102277</v>
+        <v>0.7951798759768944</v>
       </c>
       <c r="AP3">
-        <v>0.8838849069826707</v>
+        <v>0.7963849069826708</v>
       </c>
       <c r="AQ3">
-        <v>0.8892566046551138</v>
+        <v>0.7975899379884472</v>
       </c>
       <c r="AR3">
-        <v>0.894628302327557</v>
+        <v>0.7987949689942236</v>
       </c>
       <c r="AS3">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:45">
@@ -29296,76 +29296,76 @@
         <v>0.104994903160041</v>
       </c>
       <c r="V4">
-        <v>0.1025311645458522</v>
+        <v>0.1044422135633318</v>
       </c>
       <c r="W4">
-        <v>0.1000674259316635</v>
+        <v>0.1038895239666227</v>
       </c>
       <c r="X4">
-        <v>0.09760368731747469</v>
+        <v>0.1033368343699135</v>
       </c>
       <c r="Y4">
-        <v>0.09513994870328593</v>
+        <v>0.1027841447732044</v>
       </c>
       <c r="Z4">
-        <v>0.09267621008909717</v>
+        <v>0.1022314551764952</v>
       </c>
       <c r="AA4">
-        <v>0.09021247147490839</v>
+        <v>0.1016787655797861</v>
       </c>
       <c r="AB4">
-        <v>0.08774873286071963</v>
+        <v>0.1011260759830769</v>
       </c>
       <c r="AC4">
-        <v>0.08528499424653088</v>
+        <v>0.1005733863863677</v>
       </c>
       <c r="AD4">
-        <v>0.08282125563234211</v>
+        <v>0.1000206967896586</v>
       </c>
       <c r="AE4">
-        <v>0.08035751701815333</v>
+        <v>0.09946800719294943</v>
       </c>
       <c r="AF4">
-        <v>0.07789377840396458</v>
+        <v>0.09891531759624028</v>
       </c>
       <c r="AG4">
-        <v>0.0754300397897758</v>
+        <v>0.0983626279995311</v>
       </c>
       <c r="AH4">
-        <v>0.07296630117558704</v>
+        <v>0.09780993840282196</v>
       </c>
       <c r="AI4">
-        <v>0.07050256256139828</v>
+        <v>0.09725724880611281</v>
       </c>
       <c r="AJ4">
-        <v>0.0680388239472095</v>
+        <v>0.09670455920940363</v>
       </c>
       <c r="AK4">
-        <v>0.06557508533302074</v>
+        <v>0.09615186961269448</v>
       </c>
       <c r="AL4">
-        <v>0.06311134671883198</v>
+        <v>0.09559918001598533</v>
       </c>
       <c r="AM4">
-        <v>0.06064760810464322</v>
+        <v>0.09504649041927618</v>
       </c>
       <c r="AN4">
-        <v>0.05818386949045445</v>
+        <v>0.09449380082256702</v>
       </c>
       <c r="AO4">
-        <v>0.05572013087626568</v>
+        <v>0.09394111122585785</v>
       </c>
       <c r="AP4">
-        <v>0.05325639226207692</v>
+        <v>0.0933884216291487</v>
       </c>
       <c r="AQ4">
-        <v>0.05079265364788815</v>
+        <v>0.09283573203243954</v>
       </c>
       <c r="AR4">
-        <v>0.04832891503369938</v>
+        <v>0.09228304243573039</v>
       </c>
       <c r="AS4">
-        <v>0.04586517641951061</v>
+        <v>0.09173035283902123</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -29421,76 +29421,76 @@
         <v>0.121508664627931</v>
       </c>
       <c r="V5">
-        <v>0.1186574253773359</v>
+        <v>0.1208690471529045</v>
       </c>
       <c r="W5">
-        <v>0.1158061861267407</v>
+        <v>0.1202294296778779</v>
       </c>
       <c r="X5">
-        <v>0.1129549468761455</v>
+        <v>0.1195898122028514</v>
       </c>
       <c r="Y5">
-        <v>0.1101037076255504</v>
+        <v>0.1189501947278249</v>
       </c>
       <c r="Z5">
-        <v>0.1072524683749552</v>
+        <v>0.1183105772527984</v>
       </c>
       <c r="AA5">
-        <v>0.1044012291243601</v>
+        <v>0.1176709597777719</v>
       </c>
       <c r="AB5">
-        <v>0.1015499898737649</v>
+        <v>0.1170313423027454</v>
       </c>
       <c r="AC5">
-        <v>0.09869875062316977</v>
+        <v>0.1163917248277189</v>
       </c>
       <c r="AD5">
-        <v>0.09584751137257459</v>
+        <v>0.1157521073526923</v>
       </c>
       <c r="AE5">
-        <v>0.09299627212197945</v>
+        <v>0.1151124898776658</v>
       </c>
       <c r="AF5">
-        <v>0.09014503287138428</v>
+        <v>0.1144728724026393</v>
       </c>
       <c r="AG5">
-        <v>0.08729379362078914</v>
+        <v>0.1138332549276128</v>
       </c>
       <c r="AH5">
-        <v>0.08444255437019398</v>
+        <v>0.1131936374525862</v>
       </c>
       <c r="AI5">
-        <v>0.08159131511959881</v>
+        <v>0.1125540199775597</v>
       </c>
       <c r="AJ5">
-        <v>0.07874007586900367</v>
+        <v>0.1119144025025332</v>
       </c>
       <c r="AK5">
-        <v>0.07588883661840851</v>
+        <v>0.1112747850275067</v>
       </c>
       <c r="AL5">
-        <v>0.07303759736781334</v>
+        <v>0.1106351675524802</v>
       </c>
       <c r="AM5">
-        <v>0.0701863581172182</v>
+        <v>0.1099955500774537</v>
       </c>
       <c r="AN5">
-        <v>0.06733511886662305</v>
+        <v>0.1093559326024271</v>
       </c>
       <c r="AO5">
-        <v>0.06448387961602789</v>
+        <v>0.1087163151274006</v>
       </c>
       <c r="AP5">
-        <v>0.06163264036543273</v>
+        <v>0.1080766976523741</v>
       </c>
       <c r="AQ5">
-        <v>0.05878140111483758</v>
+        <v>0.1074370801773476</v>
       </c>
       <c r="AR5">
-        <v>0.05593016186424242</v>
+        <v>0.106797462702321</v>
       </c>
       <c r="AS5">
-        <v>0.05307892261364727</v>
+        <v>0.1061578452272945</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -29546,76 +29546,76 @@
         <v>0.0012085881753312</v>
       </c>
       <c r="V6">
-        <v>0.01157489700135907</v>
+        <v>0.009491563668025733</v>
       </c>
       <c r="W6">
-        <v>0.02194120582738693</v>
+        <v>0.01777453916072027</v>
       </c>
       <c r="X6">
-        <v>0.0323075146534148</v>
+        <v>0.0260575146534148</v>
       </c>
       <c r="Y6">
-        <v>0.04267382347944267</v>
+        <v>0.03434049014610933</v>
       </c>
       <c r="Z6">
-        <v>0.05304013230547053</v>
+        <v>0.04262346563880387</v>
       </c>
       <c r="AA6">
-        <v>0.0634064411314984</v>
+        <v>0.05090644113149841</v>
       </c>
       <c r="AB6">
-        <v>0.07377274995752627</v>
+        <v>0.05918941662419294</v>
       </c>
       <c r="AC6">
-        <v>0.08413905878355413</v>
+        <v>0.06747239211688746</v>
       </c>
       <c r="AD6">
-        <v>0.094505367609582</v>
+        <v>0.07575536760958201</v>
       </c>
       <c r="AE6">
-        <v>0.1048716764356099</v>
+        <v>0.08403834310227654</v>
       </c>
       <c r="AF6">
-        <v>0.1152379852616377</v>
+        <v>0.09232131859497107</v>
       </c>
       <c r="AG6">
-        <v>0.1256042940876656</v>
+        <v>0.1006042940876656</v>
       </c>
       <c r="AH6">
-        <v>0.1359706029136935</v>
+        <v>0.1088872695803601</v>
       </c>
       <c r="AI6">
-        <v>0.1463369117397214</v>
+        <v>0.1171702450730547</v>
       </c>
       <c r="AJ6">
-        <v>0.1567032205657492</v>
+        <v>0.1254532205657492</v>
       </c>
       <c r="AK6">
-        <v>0.167069529391777</v>
+        <v>0.1337361960584437</v>
       </c>
       <c r="AL6">
-        <v>0.177435838217805</v>
+        <v>0.1420191715511383</v>
       </c>
       <c r="AM6">
-        <v>0.1878021470438328</v>
+        <v>0.1503021470438328</v>
       </c>
       <c r="AN6">
-        <v>0.1981684558698606</v>
+        <v>0.1585851225365273</v>
       </c>
       <c r="AO6">
-        <v>0.2085347646958886</v>
+        <v>0.1668680980292219</v>
       </c>
       <c r="AP6">
-        <v>0.2189010735219164</v>
+        <v>0.1751510735219164</v>
       </c>
       <c r="AQ6">
-        <v>0.2292673823479442</v>
+        <v>0.1834340490146109</v>
       </c>
       <c r="AR6">
-        <v>0.2396336911739722</v>
+        <v>0.1917170245073055</v>
       </c>
       <c r="AS6">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -29671,76 +29671,76 @@
         <v>0.0012085881753312</v>
       </c>
       <c r="V7">
-        <v>0.01157489700135907</v>
+        <v>0.009491563668025733</v>
       </c>
       <c r="W7">
-        <v>0.02194120582738693</v>
+        <v>0.01777453916072027</v>
       </c>
       <c r="X7">
-        <v>0.0323075146534148</v>
+        <v>0.0260575146534148</v>
       </c>
       <c r="Y7">
-        <v>0.04267382347944267</v>
+        <v>0.03434049014610933</v>
       </c>
       <c r="Z7">
-        <v>0.05304013230547053</v>
+        <v>0.04262346563880387</v>
       </c>
       <c r="AA7">
-        <v>0.0634064411314984</v>
+        <v>0.05090644113149841</v>
       </c>
       <c r="AB7">
-        <v>0.07377274995752627</v>
+        <v>0.05918941662419294</v>
       </c>
       <c r="AC7">
-        <v>0.08413905878355413</v>
+        <v>0.06747239211688746</v>
       </c>
       <c r="AD7">
-        <v>0.094505367609582</v>
+        <v>0.07575536760958201</v>
       </c>
       <c r="AE7">
-        <v>0.1048716764356099</v>
+        <v>0.08403834310227654</v>
       </c>
       <c r="AF7">
-        <v>0.1152379852616377</v>
+        <v>0.09232131859497107</v>
       </c>
       <c r="AG7">
-        <v>0.1256042940876656</v>
+        <v>0.1006042940876656</v>
       </c>
       <c r="AH7">
-        <v>0.1359706029136935</v>
+        <v>0.1088872695803601</v>
       </c>
       <c r="AI7">
-        <v>0.1463369117397214</v>
+        <v>0.1171702450730547</v>
       </c>
       <c r="AJ7">
-        <v>0.1567032205657492</v>
+        <v>0.1254532205657492</v>
       </c>
       <c r="AK7">
-        <v>0.167069529391777</v>
+        <v>0.1337361960584437</v>
       </c>
       <c r="AL7">
-        <v>0.177435838217805</v>
+        <v>0.1420191715511383</v>
       </c>
       <c r="AM7">
-        <v>0.1878021470438328</v>
+        <v>0.1503021470438328</v>
       </c>
       <c r="AN7">
-        <v>0.1981684558698606</v>
+        <v>0.1585851225365273</v>
       </c>
       <c r="AO7">
-        <v>0.2085347646958886</v>
+        <v>0.1668680980292219</v>
       </c>
       <c r="AP7">
-        <v>0.2189010735219164</v>
+        <v>0.1751510735219164</v>
       </c>
       <c r="AQ7">
-        <v>0.2292673823479442</v>
+        <v>0.1834340490146109</v>
       </c>
       <c r="AR7">
-        <v>0.2396336911739722</v>
+        <v>0.1917170245073055</v>
       </c>
       <c r="AS7">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -30046,76 +30046,76 @@
         <v>0.104994903160041</v>
       </c>
       <c r="V10">
-        <v>0.1025515586726871</v>
+        <v>0.1044830018170015</v>
       </c>
       <c r="W10">
-        <v>0.1001082141853331</v>
+        <v>0.103971100473962</v>
       </c>
       <c r="X10">
-        <v>0.09766486969797918</v>
+        <v>0.1034591991309225</v>
       </c>
       <c r="Y10">
-        <v>0.09522152521062524</v>
+        <v>0.102947297787883</v>
       </c>
       <c r="Z10">
-        <v>0.09277818072327131</v>
+        <v>0.1024353964448435</v>
       </c>
       <c r="AA10">
-        <v>0.09033483623591736</v>
+        <v>0.101923495101804</v>
       </c>
       <c r="AB10">
-        <v>0.08789149174856342</v>
+        <v>0.1014115937587644</v>
       </c>
       <c r="AC10">
-        <v>0.0854481472612095</v>
+        <v>0.100899692415725</v>
       </c>
       <c r="AD10">
-        <v>0.08300480277385555</v>
+        <v>0.1003877910726854</v>
       </c>
       <c r="AE10">
-        <v>0.0805614582865016</v>
+        <v>0.09987588972964594</v>
       </c>
       <c r="AF10">
-        <v>0.07811811379914768</v>
+        <v>0.09936398838660643</v>
       </c>
       <c r="AG10">
-        <v>0.07567476931179373</v>
+        <v>0.09885208704356693</v>
       </c>
       <c r="AH10">
-        <v>0.0732314248244398</v>
+        <v>0.09834018570052742</v>
       </c>
       <c r="AI10">
-        <v>0.07078808033708586</v>
+        <v>0.09782828435748792</v>
       </c>
       <c r="AJ10">
-        <v>0.06834473584973191</v>
+        <v>0.09731638301444841</v>
       </c>
       <c r="AK10">
-        <v>0.06590139136237799</v>
+        <v>0.0968044816714089</v>
       </c>
       <c r="AL10">
-        <v>0.06345804687502404</v>
+        <v>0.0962925803283694</v>
       </c>
       <c r="AM10">
-        <v>0.06101470238767011</v>
+        <v>0.0957806789853299</v>
       </c>
       <c r="AN10">
-        <v>0.05857135790031617</v>
+        <v>0.09526877764229039</v>
       </c>
       <c r="AO10">
-        <v>0.05612801341296222</v>
+        <v>0.09475687629925089</v>
       </c>
       <c r="AP10">
-        <v>0.0536846689256083</v>
+        <v>0.09424497495621137</v>
       </c>
       <c r="AQ10">
-        <v>0.05124132443825435</v>
+        <v>0.09373307361317186</v>
       </c>
       <c r="AR10">
-        <v>0.04879797995090041</v>
+        <v>0.09322117227013237</v>
       </c>
       <c r="AS10">
-        <v>0.04635463546354648</v>
+        <v>0.09270927092709286</v>
       </c>
     </row>
     <row r="11" spans="1:45">
@@ -30171,76 +30171,76 @@
         <v>0.121508664627931</v>
       </c>
       <c r="V11">
-        <v>0.1186810271241195</v>
+        <v>0.1209162506464717</v>
       </c>
       <c r="W11">
-        <v>0.1158533896203079</v>
+        <v>0.1203238366650124</v>
       </c>
       <c r="X11">
-        <v>0.1130257521164964</v>
+        <v>0.1197314226835531</v>
       </c>
       <c r="Y11">
-        <v>0.1101981146126848</v>
+        <v>0.1191390087020937</v>
       </c>
       <c r="Z11">
-        <v>0.1073704771088732</v>
+        <v>0.1185465947206344</v>
       </c>
       <c r="AA11">
-        <v>0.1045428396050617</v>
+        <v>0.1179541807391751</v>
       </c>
       <c r="AB11">
-        <v>0.1017152021012502</v>
+        <v>0.1173617667577158</v>
       </c>
       <c r="AC11">
-        <v>0.09888756459743862</v>
+        <v>0.1167693527762565</v>
       </c>
       <c r="AD11">
-        <v>0.09605992709362705</v>
+        <v>0.1161769387947972</v>
       </c>
       <c r="AE11">
-        <v>0.0932322895898155</v>
+        <v>0.1155845248133379</v>
       </c>
       <c r="AF11">
-        <v>0.09040465208600396</v>
+        <v>0.1149921108318786</v>
       </c>
       <c r="AG11">
-        <v>0.08757701458219241</v>
+        <v>0.1143996968504193</v>
       </c>
       <c r="AH11">
-        <v>0.08474937707838086</v>
+        <v>0.1138072828689599</v>
       </c>
       <c r="AI11">
-        <v>0.0819217395745693</v>
+        <v>0.1132148688875006</v>
       </c>
       <c r="AJ11">
-        <v>0.07909410207075776</v>
+        <v>0.1126224549060413</v>
       </c>
       <c r="AK11">
-        <v>0.07626646456694622</v>
+        <v>0.112030040924582</v>
       </c>
       <c r="AL11">
-        <v>0.07343882706313466</v>
+        <v>0.1114376269431227</v>
       </c>
       <c r="AM11">
-        <v>0.07061118955932311</v>
+        <v>0.1108452129616634</v>
       </c>
       <c r="AN11">
-        <v>0.06778355205551156</v>
+        <v>0.1102527989802041</v>
       </c>
       <c r="AO11">
-        <v>0.06495591455170001</v>
+        <v>0.1096603849987448</v>
       </c>
       <c r="AP11">
-        <v>0.06212827704788847</v>
+        <v>0.1090679710172855</v>
       </c>
       <c r="AQ11">
-        <v>0.05930063954407692</v>
+        <v>0.1084755570358261</v>
       </c>
       <c r="AR11">
-        <v>0.05647300204026537</v>
+        <v>0.1078831430543668</v>
       </c>
       <c r="AS11">
-        <v>0.05364536453645382</v>
+        <v>0.1072907290729075</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -30296,76 +30296,76 @@
         <v>0.0012085881753312</v>
       </c>
       <c r="V12">
-        <v>0.001180345026121924</v>
+        <v>0.001202459717551447</v>
       </c>
       <c r="W12">
-        <v>0.001152101876912647</v>
+        <v>0.001196331259771695</v>
       </c>
       <c r="X12">
-        <v>0.001123858727703371</v>
+        <v>0.001190202801991942</v>
       </c>
       <c r="Y12">
-        <v>0.001095615578494095</v>
+        <v>0.001184074344212189</v>
       </c>
       <c r="Z12">
-        <v>0.001067372429284818</v>
+        <v>0.001177945886432436</v>
       </c>
       <c r="AA12">
-        <v>0.001039129280075542</v>
+        <v>0.001171817428652684</v>
       </c>
       <c r="AB12">
-        <v>0.001010886130866266</v>
+        <v>0.001165688970872931</v>
       </c>
       <c r="AC12">
-        <v>0.0009826429816569894</v>
+        <v>0.001159560513093178</v>
       </c>
       <c r="AD12">
-        <v>0.000954399832447713</v>
+        <v>0.001153432055313426</v>
       </c>
       <c r="AE12">
-        <v>0.0009261566832384366</v>
+        <v>0.001147303597533673</v>
       </c>
       <c r="AF12">
-        <v>0.0008979135340291604</v>
+        <v>0.00114117513975392</v>
       </c>
       <c r="AG12">
-        <v>0.000869670384819884</v>
+        <v>0.001135046681974167</v>
       </c>
       <c r="AH12">
-        <v>0.0008414272356106076</v>
+        <v>0.001128918224194414</v>
       </c>
       <c r="AI12">
-        <v>0.0008131840864013312</v>
+        <v>0.001122789766414662</v>
       </c>
       <c r="AJ12">
-        <v>0.0007849409371920549</v>
+        <v>0.001116661308634909</v>
       </c>
       <c r="AK12">
-        <v>0.0007566977879827786</v>
+        <v>0.001110532850855156</v>
       </c>
       <c r="AL12">
-        <v>0.0007284546387735021</v>
+        <v>0.001104404393075403</v>
       </c>
       <c r="AM12">
-        <v>0.0007002114895642258</v>
+        <v>0.001098275935295651</v>
       </c>
       <c r="AN12">
-        <v>0.0006719683403549495</v>
+        <v>0.001092147477515898</v>
       </c>
       <c r="AO12">
-        <v>0.0006437251911456731</v>
+        <v>0.001086019019736145</v>
       </c>
       <c r="AP12">
-        <v>0.0006154820419363967</v>
+        <v>0.001079890561956392</v>
       </c>
       <c r="AQ12">
-        <v>0.0005872388927271204</v>
+        <v>0.00107376210417664</v>
       </c>
       <c r="AR12">
-        <v>0.0005589957435178441</v>
+        <v>0.001067633646396887</v>
       </c>
       <c r="AS12">
-        <v>0.0005307525943085677</v>
+        <v>0.001061505188617134</v>
       </c>
     </row>
     <row r="13" spans="1:45">
@@ -30421,76 +30421,76 @@
         <v>0.0012085881753312</v>
       </c>
       <c r="V13">
-        <v>0.02199156366802573</v>
+        <v>0.01782489700135906</v>
       </c>
       <c r="W13">
-        <v>0.04277453916072026</v>
+        <v>0.03444120582738693</v>
       </c>
       <c r="X13">
-        <v>0.0635575146534148</v>
+        <v>0.0510575146534148</v>
       </c>
       <c r="Y13">
-        <v>0.08434049014610932</v>
+        <v>0.06767382347944266</v>
       </c>
       <c r="Z13">
-        <v>0.1051234656388039</v>
+        <v>0.08429013230547054</v>
       </c>
       <c r="AA13">
-        <v>0.1259064411314984</v>
+        <v>0.1009064411314984</v>
       </c>
       <c r="AB13">
-        <v>0.1466894166241929</v>
+        <v>0.1175227499575263</v>
       </c>
       <c r="AC13">
-        <v>0.1674723921168875</v>
+        <v>0.1341390587835541</v>
       </c>
       <c r="AD13">
-        <v>0.188255367609582</v>
+        <v>0.150755367609582</v>
       </c>
       <c r="AE13">
-        <v>0.2090383431022765</v>
+        <v>0.1673716764356099</v>
       </c>
       <c r="AF13">
-        <v>0.2298213185949711</v>
+        <v>0.1839879852616378</v>
       </c>
       <c r="AG13">
-        <v>0.2506042940876656</v>
+        <v>0.2006042940876656</v>
       </c>
       <c r="AH13">
-        <v>0.2713872695803601</v>
+        <v>0.2172206029136935</v>
       </c>
       <c r="AI13">
-        <v>0.2921702450730547</v>
+        <v>0.2338369117397214</v>
       </c>
       <c r="AJ13">
-        <v>0.3129532205657492</v>
+        <v>0.2504532205657492</v>
       </c>
       <c r="AK13">
-        <v>0.3337361960584437</v>
+        <v>0.2670695293917771</v>
       </c>
       <c r="AL13">
-        <v>0.3545191715511383</v>
+        <v>0.283685838217805</v>
       </c>
       <c r="AM13">
-        <v>0.3753021470438328</v>
+        <v>0.3003021470438328</v>
       </c>
       <c r="AN13">
-        <v>0.3960851225365273</v>
+        <v>0.3169184558698607</v>
       </c>
       <c r="AO13">
-        <v>0.4168680980292219</v>
+        <v>0.3335347646958886</v>
       </c>
       <c r="AP13">
-        <v>0.4376510735219164</v>
+        <v>0.3501510735219164</v>
       </c>
       <c r="AQ13">
-        <v>0.4584340490146109</v>
+        <v>0.3667673823479443</v>
       </c>
       <c r="AR13">
-        <v>0.4792170245073055</v>
+        <v>0.3833836911739721</v>
       </c>
       <c r="AS13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -30796,76 +30796,76 @@
         <v>0.104994903160041</v>
       </c>
       <c r="V16">
-        <v>0.102541307488091</v>
+        <v>0.1044624994478094</v>
       </c>
       <c r="W16">
-        <v>0.100087711816141</v>
+        <v>0.1039300957355778</v>
       </c>
       <c r="X16">
-        <v>0.09763411614419104</v>
+        <v>0.1033976920233462</v>
       </c>
       <c r="Y16">
-        <v>0.09518052047224107</v>
+        <v>0.1028652883111146</v>
       </c>
       <c r="Z16">
-        <v>0.09272692480029109</v>
+        <v>0.102332884598883</v>
       </c>
       <c r="AA16">
-        <v>0.0902733291283411</v>
+        <v>0.1018004808866514</v>
       </c>
       <c r="AB16">
-        <v>0.08781973345639112</v>
+        <v>0.1012680771744198</v>
       </c>
       <c r="AC16">
-        <v>0.08536613778444115</v>
+        <v>0.1007356734621883</v>
       </c>
       <c r="AD16">
-        <v>0.08291254211249115</v>
+        <v>0.1002032697499566</v>
       </c>
       <c r="AE16">
-        <v>0.08045894644054116</v>
+        <v>0.09967086603772504</v>
       </c>
       <c r="AF16">
-        <v>0.07800535076859119</v>
+        <v>0.09913846232549348</v>
       </c>
       <c r="AG16">
-        <v>0.07555175509664121</v>
+        <v>0.09860605861326187</v>
       </c>
       <c r="AH16">
-        <v>0.07309815942469124</v>
+        <v>0.09807365490103027</v>
       </c>
       <c r="AI16">
-        <v>0.07064456375274125</v>
+        <v>0.09754125118879868</v>
       </c>
       <c r="AJ16">
-        <v>0.06819096808079127</v>
+        <v>0.09700884747656709</v>
       </c>
       <c r="AK16">
-        <v>0.06573737240884128</v>
+        <v>0.09647644376433549</v>
       </c>
       <c r="AL16">
-        <v>0.0632837767368913</v>
+        <v>0.09594404005210391</v>
       </c>
       <c r="AM16">
-        <v>0.06083018106494131</v>
+        <v>0.0954116363398723</v>
       </c>
       <c r="AN16">
-        <v>0.05837658539299134</v>
+        <v>0.09487923262764071</v>
       </c>
       <c r="AO16">
-        <v>0.05592298972104135</v>
+        <v>0.0943468289154091</v>
       </c>
       <c r="AP16">
-        <v>0.05346939404909137</v>
+        <v>0.09381442520317752</v>
       </c>
       <c r="AQ16">
-        <v>0.05101579837714139</v>
+        <v>0.09328202149094593</v>
       </c>
       <c r="AR16">
-        <v>0.0485622027051914</v>
+        <v>0.09274961777871434</v>
       </c>
       <c r="AS16">
-        <v>0.04610860703324143</v>
+        <v>0.09221721406648274</v>
       </c>
     </row>
     <row r="17" spans="1:45">
@@ -30921,76 +30921,76 @@
         <v>0.121508664627931</v>
       </c>
       <c r="V17">
-        <v>0.118669163617286</v>
+        <v>0.1208925236328047</v>
       </c>
       <c r="W17">
-        <v>0.1158296626066409</v>
+        <v>0.1202763826376785</v>
       </c>
       <c r="X17">
-        <v>0.1129901615959959</v>
+        <v>0.1196602416425522</v>
       </c>
       <c r="Y17">
-        <v>0.1101506605853509</v>
+        <v>0.1190441006474259</v>
       </c>
       <c r="Z17">
-        <v>0.1073111595747059</v>
+        <v>0.1184279596522996</v>
       </c>
       <c r="AA17">
-        <v>0.1044716585640608</v>
+        <v>0.1178118186571734</v>
       </c>
       <c r="AB17">
-        <v>0.1016321575534158</v>
+        <v>0.1171956776620471</v>
       </c>
       <c r="AC17">
-        <v>0.09879265654277078</v>
+        <v>0.1165795366669208</v>
       </c>
       <c r="AD17">
-        <v>0.09595315553212573</v>
+        <v>0.1159633956717945</v>
       </c>
       <c r="AE17">
-        <v>0.0931136545214807</v>
+        <v>0.1153472546766683</v>
       </c>
       <c r="AF17">
-        <v>0.09027415351083568</v>
+        <v>0.114731113681542</v>
       </c>
       <c r="AG17">
-        <v>0.08743465250019064</v>
+        <v>0.1141149726864157</v>
       </c>
       <c r="AH17">
-        <v>0.08459515148954562</v>
+        <v>0.1134988316912895</v>
       </c>
       <c r="AI17">
-        <v>0.08175565047890059</v>
+        <v>0.1128826906961632</v>
       </c>
       <c r="AJ17">
-        <v>0.07891614946825556</v>
+        <v>0.1122665497010369</v>
       </c>
       <c r="AK17">
-        <v>0.07607664845761053</v>
+        <v>0.1116504087059106</v>
       </c>
       <c r="AL17">
-        <v>0.07323714744696549</v>
+        <v>0.1110342677107844</v>
       </c>
       <c r="AM17">
-        <v>0.07039764643632046</v>
+        <v>0.1104181267156581</v>
       </c>
       <c r="AN17">
-        <v>0.06755814542567544</v>
+        <v>0.1098019857205318</v>
       </c>
       <c r="AO17">
-        <v>0.0647186444150304</v>
+        <v>0.1091858447254056</v>
       </c>
       <c r="AP17">
-        <v>0.06187914340438538</v>
+        <v>0.1085697037302793</v>
       </c>
       <c r="AQ17">
-        <v>0.05903964239374036</v>
+        <v>0.107953562735153</v>
       </c>
       <c r="AR17">
-        <v>0.05620014138309532</v>
+        <v>0.1073374217400267</v>
       </c>
       <c r="AS17">
-        <v>0.05336064037245029</v>
+        <v>0.1067212807449005</v>
       </c>
     </row>
     <row r="18" spans="1:45">
@@ -31321,76 +31321,76 @@
         <v>0.0024171763506625</v>
       </c>
       <c r="V2">
-        <v>0.002316460669384896</v>
+        <v>0.002360456543003326</v>
       </c>
       <c r="W2">
-        <v>0.002215744988107292</v>
+        <v>0.002303736735344153</v>
       </c>
       <c r="X2">
-        <v>0.002115029306829688</v>
+        <v>0.002247016927684979</v>
       </c>
       <c r="Y2">
-        <v>0.002014313625552083</v>
+        <v>0.002190297120025806</v>
       </c>
       <c r="Z2">
-        <v>0.001913597944274479</v>
+        <v>0.002133577312366632</v>
       </c>
       <c r="AA2">
-        <v>0.001812882262996875</v>
+        <v>0.002076857504707458</v>
       </c>
       <c r="AB2">
-        <v>0.001712166581719271</v>
+        <v>0.002020137697048285</v>
       </c>
       <c r="AC2">
-        <v>0.001611450900441667</v>
+        <v>0.001963417889389111</v>
       </c>
       <c r="AD2">
-        <v>0.001510735219164062</v>
+        <v>0.001906698081729937</v>
       </c>
       <c r="AE2">
-        <v>0.001410019537886458</v>
+        <v>0.001849978274070764</v>
       </c>
       <c r="AF2">
-        <v>0.001309303856608854</v>
+        <v>0.00179325846641159</v>
       </c>
       <c r="AG2">
-        <v>0.00120858817533125</v>
+        <v>0.001736538658752416</v>
       </c>
       <c r="AH2">
-        <v>0.001107872494053646</v>
+        <v>0.001679818851093243</v>
       </c>
       <c r="AI2">
-        <v>0.001007156812776042</v>
+        <v>0.001623099043434069</v>
       </c>
       <c r="AJ2">
-        <v>0.0009064411314984375</v>
+        <v>0.001566379235774896</v>
       </c>
       <c r="AK2">
-        <v>0.0008057254502208334</v>
+        <v>0.001509659428115722</v>
       </c>
       <c r="AL2">
-        <v>0.0007050097689432291</v>
+        <v>0.001452939620456548</v>
       </c>
       <c r="AM2">
-        <v>0.000604294087665625</v>
+        <v>0.001396219812797375</v>
       </c>
       <c r="AN2">
-        <v>0.0005035784063880209</v>
+        <v>0.001339500005138201</v>
       </c>
       <c r="AO2">
-        <v>0.0004028627251104166</v>
+        <v>0.001282780197479027</v>
       </c>
       <c r="AP2">
-        <v>0.0003021470438328125</v>
+        <v>0.001226060389819854</v>
       </c>
       <c r="AQ2">
-        <v>0.0002014313625552084</v>
+        <v>0.00116934058216068</v>
       </c>
       <c r="AR2">
-        <v>0.0001007156812776041</v>
+        <v>0.001112620774501507</v>
       </c>
       <c r="AS2">
-        <v>0</v>
+        <v>0.001055900966842333</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -31446,76 +31446,76 @@
         <v>0.7710792558613661</v>
       </c>
       <c r="V3">
-        <v>0.7806176202004758</v>
+        <v>0.7764509535338091</v>
       </c>
       <c r="W3">
-        <v>0.7901559845395856</v>
+        <v>0.7818226512062522</v>
       </c>
       <c r="X3">
-        <v>0.7996943488786953</v>
+        <v>0.7871943488786953</v>
       </c>
       <c r="Y3">
-        <v>0.809232713217805</v>
+        <v>0.7925660465511384</v>
       </c>
       <c r="Z3">
-        <v>0.8187710775569148</v>
+        <v>0.7979377442235814</v>
       </c>
       <c r="AA3">
-        <v>0.8283094418960245</v>
+        <v>0.8033094418960245</v>
       </c>
       <c r="AB3">
-        <v>0.8378478062351342</v>
+        <v>0.8086811395684677</v>
       </c>
       <c r="AC3">
-        <v>0.847386170574244</v>
+        <v>0.8140528372409108</v>
       </c>
       <c r="AD3">
-        <v>0.8569245349133539</v>
+        <v>0.8194245349133538</v>
       </c>
       <c r="AE3">
-        <v>0.8664628992524634</v>
+        <v>0.8247962325857968</v>
       </c>
       <c r="AF3">
-        <v>0.8760012635915733</v>
+        <v>0.83016793025824</v>
       </c>
       <c r="AG3">
-        <v>0.8855396279306831</v>
+        <v>0.835539627930683</v>
       </c>
       <c r="AH3">
-        <v>0.8950779922697928</v>
+        <v>0.8409113256031262</v>
       </c>
       <c r="AI3">
-        <v>0.9046163566089025</v>
+        <v>0.8462830232755691</v>
       </c>
       <c r="AJ3">
-        <v>0.9141547209480123</v>
+        <v>0.8516547209480123</v>
       </c>
       <c r="AK3">
-        <v>0.923693085287122</v>
+        <v>0.8570264186204554</v>
       </c>
       <c r="AL3">
-        <v>0.9332314496262317</v>
+        <v>0.8623981162928984</v>
       </c>
       <c r="AM3">
-        <v>0.9427698139653415</v>
+        <v>0.8677698139653416</v>
       </c>
       <c r="AN3">
-        <v>0.9523081783044512</v>
+        <v>0.8731415116377846</v>
       </c>
       <c r="AO3">
-        <v>0.961846542643561</v>
+        <v>0.8785132093102277</v>
       </c>
       <c r="AP3">
-        <v>0.9713849069826708</v>
+        <v>0.8838849069826707</v>
       </c>
       <c r="AQ3">
-        <v>0.9809232713217805</v>
+        <v>0.8892566046551138</v>
       </c>
       <c r="AR3">
-        <v>0.9904616356608903</v>
+        <v>0.894628302327557</v>
       </c>
       <c r="AS3">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:45">
@@ -31571,76 +31571,76 @@
         <v>0.104994903160041</v>
       </c>
       <c r="V4">
-        <v>0.1006201155283726</v>
+        <v>0.1025311645458522</v>
       </c>
       <c r="W4">
-        <v>0.09624532789670424</v>
+        <v>0.1000674259316635</v>
       </c>
       <c r="X4">
-        <v>0.09187054026503587</v>
+        <v>0.09760368731747469</v>
       </c>
       <c r="Y4">
-        <v>0.08749575263336749</v>
+        <v>0.09513994870328593</v>
       </c>
       <c r="Z4">
-        <v>0.08312096500169912</v>
+        <v>0.09267621008909717</v>
       </c>
       <c r="AA4">
-        <v>0.07874617737003074</v>
+        <v>0.09021247147490839</v>
       </c>
       <c r="AB4">
-        <v>0.07437138973836237</v>
+        <v>0.08774873286071963</v>
       </c>
       <c r="AC4">
-        <v>0.06999660210669401</v>
+        <v>0.08528499424653088</v>
       </c>
       <c r="AD4">
-        <v>0.06562181447502562</v>
+        <v>0.08282125563234211</v>
       </c>
       <c r="AE4">
-        <v>0.06124702684335724</v>
+        <v>0.08035751701815333</v>
       </c>
       <c r="AF4">
-        <v>0.05687223921168888</v>
+        <v>0.07789377840396458</v>
       </c>
       <c r="AG4">
-        <v>0.0524974515800205</v>
+        <v>0.0754300397897758</v>
       </c>
       <c r="AH4">
-        <v>0.04812266394835213</v>
+        <v>0.07296630117558704</v>
       </c>
       <c r="AI4">
-        <v>0.04374787631668375</v>
+        <v>0.07050256256139828</v>
       </c>
       <c r="AJ4">
-        <v>0.03937308868501537</v>
+        <v>0.0680388239472095</v>
       </c>
       <c r="AK4">
-        <v>0.034998301053347</v>
+        <v>0.06557508533302074</v>
       </c>
       <c r="AL4">
-        <v>0.03062351342167862</v>
+        <v>0.06311134671883198</v>
       </c>
       <c r="AM4">
-        <v>0.02624872579001025</v>
+        <v>0.06064760810464322</v>
       </c>
       <c r="AN4">
-        <v>0.02187393815834188</v>
+        <v>0.05818386949045445</v>
       </c>
       <c r="AO4">
-        <v>0.01749915052667349</v>
+        <v>0.05572013087626568</v>
       </c>
       <c r="AP4">
-        <v>0.01312436289500512</v>
+        <v>0.05325639226207692</v>
       </c>
       <c r="AQ4">
-        <v>0.008749575263336754</v>
+        <v>0.05079265364788815</v>
       </c>
       <c r="AR4">
-        <v>0.004374787631668371</v>
+        <v>0.04832891503369938</v>
       </c>
       <c r="AS4">
-        <v>0</v>
+        <v>0.04586517641951061</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -31696,76 +31696,76 @@
         <v>0.121508664627931</v>
       </c>
       <c r="V5">
-        <v>0.1164458036017672</v>
+        <v>0.1186574253773359</v>
       </c>
       <c r="W5">
-        <v>0.1113829425756034</v>
+        <v>0.1158061861267407</v>
       </c>
       <c r="X5">
-        <v>0.1063200815494396</v>
+        <v>0.1129549468761455</v>
       </c>
       <c r="Y5">
-        <v>0.1012572205232758</v>
+        <v>0.1101037076255504</v>
       </c>
       <c r="Z5">
-        <v>0.09619435949711204</v>
+        <v>0.1072524683749552</v>
       </c>
       <c r="AA5">
-        <v>0.09113149847094826</v>
+        <v>0.1044012291243601</v>
       </c>
       <c r="AB5">
-        <v>0.08606863744478445</v>
+        <v>0.1015499898737649</v>
       </c>
       <c r="AC5">
-        <v>0.08100577641862068</v>
+        <v>0.09869875062316977</v>
       </c>
       <c r="AD5">
-        <v>0.07594291539245687</v>
+        <v>0.09584751137257459</v>
       </c>
       <c r="AE5">
-        <v>0.07088005436629308</v>
+        <v>0.09299627212197945</v>
       </c>
       <c r="AF5">
-        <v>0.0658171933401293</v>
+        <v>0.09014503287138428</v>
       </c>
       <c r="AG5">
-        <v>0.0607543323139655</v>
+        <v>0.08729379362078914</v>
       </c>
       <c r="AH5">
-        <v>0.05569147128780171</v>
+        <v>0.08444255437019398</v>
       </c>
       <c r="AI5">
-        <v>0.05062861026163791</v>
+        <v>0.08159131511959881</v>
       </c>
       <c r="AJ5">
-        <v>0.04556574923547413</v>
+        <v>0.07874007586900367</v>
       </c>
       <c r="AK5">
-        <v>0.04050288820931034</v>
+        <v>0.07588883661840851</v>
       </c>
       <c r="AL5">
-        <v>0.03544002718314654</v>
+        <v>0.07303759736781334</v>
       </c>
       <c r="AM5">
-        <v>0.03037716615698275</v>
+        <v>0.0701863581172182</v>
       </c>
       <c r="AN5">
-        <v>0.02531430513081896</v>
+        <v>0.06733511886662305</v>
       </c>
       <c r="AO5">
-        <v>0.02025144410465516</v>
+        <v>0.06448387961602789</v>
       </c>
       <c r="AP5">
-        <v>0.01518858307849138</v>
+        <v>0.06163264036543273</v>
       </c>
       <c r="AQ5">
-        <v>0.01012572205232759</v>
+        <v>0.05878140111483758</v>
       </c>
       <c r="AR5">
-        <v>0.005062861026163787</v>
+        <v>0.05593016186424242</v>
       </c>
       <c r="AS5">
-        <v>0</v>
+        <v>0.05307892261364727</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -31821,76 +31821,76 @@
         <v>0.0012085881753312</v>
       </c>
       <c r="V6">
-        <v>0.0136582303346924</v>
+        <v>0.01157489700135907</v>
       </c>
       <c r="W6">
-        <v>0.0261078724940536</v>
+        <v>0.02194120582738693</v>
       </c>
       <c r="X6">
-        <v>0.0385575146534148</v>
+        <v>0.0323075146534148</v>
       </c>
       <c r="Y6">
-        <v>0.051007156812776</v>
+        <v>0.04267382347944267</v>
       </c>
       <c r="Z6">
-        <v>0.0634567989721372</v>
+        <v>0.05304013230547053</v>
       </c>
       <c r="AA6">
-        <v>0.0759064411314984</v>
+        <v>0.0634064411314984</v>
       </c>
       <c r="AB6">
-        <v>0.0883560832908596</v>
+        <v>0.07377274995752627</v>
       </c>
       <c r="AC6">
-        <v>0.1008057254502208</v>
+        <v>0.08413905878355413</v>
       </c>
       <c r="AD6">
-        <v>0.113255367609582</v>
+        <v>0.094505367609582</v>
       </c>
       <c r="AE6">
-        <v>0.1257050097689432</v>
+        <v>0.1048716764356099</v>
       </c>
       <c r="AF6">
-        <v>0.1381546519283044</v>
+        <v>0.1152379852616377</v>
       </c>
       <c r="AG6">
-        <v>0.1506042940876656</v>
+        <v>0.1256042940876656</v>
       </c>
       <c r="AH6">
-        <v>0.1630539362470268</v>
+        <v>0.1359706029136935</v>
       </c>
       <c r="AI6">
-        <v>0.175503578406388</v>
+        <v>0.1463369117397214</v>
       </c>
       <c r="AJ6">
-        <v>0.1879532205657492</v>
+        <v>0.1567032205657492</v>
       </c>
       <c r="AK6">
-        <v>0.2004028627251104</v>
+        <v>0.167069529391777</v>
       </c>
       <c r="AL6">
-        <v>0.2128525048844716</v>
+        <v>0.177435838217805</v>
       </c>
       <c r="AM6">
-        <v>0.2253021470438328</v>
+        <v>0.1878021470438328</v>
       </c>
       <c r="AN6">
-        <v>0.237751789203194</v>
+        <v>0.1981684558698606</v>
       </c>
       <c r="AO6">
-        <v>0.2502014313625552</v>
+        <v>0.2085347646958886</v>
       </c>
       <c r="AP6">
-        <v>0.2626510735219164</v>
+        <v>0.2189010735219164</v>
       </c>
       <c r="AQ6">
-        <v>0.2751007156812776</v>
+        <v>0.2292673823479442</v>
       </c>
       <c r="AR6">
-        <v>0.2875503578406388</v>
+        <v>0.2396336911739722</v>
       </c>
       <c r="AS6">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -31946,76 +31946,76 @@
         <v>0.0012085881753312</v>
       </c>
       <c r="V7">
-        <v>0.0136582303346924</v>
+        <v>0.01157489700135907</v>
       </c>
       <c r="W7">
-        <v>0.0261078724940536</v>
+        <v>0.02194120582738693</v>
       </c>
       <c r="X7">
-        <v>0.0385575146534148</v>
+        <v>0.0323075146534148</v>
       </c>
       <c r="Y7">
-        <v>0.051007156812776</v>
+        <v>0.04267382347944267</v>
       </c>
       <c r="Z7">
-        <v>0.0634567989721372</v>
+        <v>0.05304013230547053</v>
       </c>
       <c r="AA7">
-        <v>0.0759064411314984</v>
+        <v>0.0634064411314984</v>
       </c>
       <c r="AB7">
-        <v>0.0883560832908596</v>
+        <v>0.07377274995752627</v>
       </c>
       <c r="AC7">
-        <v>0.1008057254502208</v>
+        <v>0.08413905878355413</v>
       </c>
       <c r="AD7">
-        <v>0.113255367609582</v>
+        <v>0.094505367609582</v>
       </c>
       <c r="AE7">
-        <v>0.1257050097689432</v>
+        <v>0.1048716764356099</v>
       </c>
       <c r="AF7">
-        <v>0.1381546519283044</v>
+        <v>0.1152379852616377</v>
       </c>
       <c r="AG7">
-        <v>0.1506042940876656</v>
+        <v>0.1256042940876656</v>
       </c>
       <c r="AH7">
-        <v>0.1630539362470268</v>
+        <v>0.1359706029136935</v>
       </c>
       <c r="AI7">
-        <v>0.175503578406388</v>
+        <v>0.1463369117397214</v>
       </c>
       <c r="AJ7">
-        <v>0.1879532205657492</v>
+        <v>0.1567032205657492</v>
       </c>
       <c r="AK7">
-        <v>0.2004028627251104</v>
+        <v>0.167069529391777</v>
       </c>
       <c r="AL7">
-        <v>0.2128525048844716</v>
+        <v>0.177435838217805</v>
       </c>
       <c r="AM7">
-        <v>0.2253021470438328</v>
+        <v>0.1878021470438328</v>
       </c>
       <c r="AN7">
-        <v>0.237751789203194</v>
+        <v>0.1981684558698606</v>
       </c>
       <c r="AO7">
-        <v>0.2502014313625552</v>
+        <v>0.2085347646958886</v>
       </c>
       <c r="AP7">
-        <v>0.2626510735219164</v>
+        <v>0.2189010735219164</v>
       </c>
       <c r="AQ7">
-        <v>0.2751007156812776</v>
+        <v>0.2292673823479442</v>
       </c>
       <c r="AR7">
-        <v>0.2875503578406388</v>
+        <v>0.2396336911739722</v>
       </c>
       <c r="AS7">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -32321,76 +32321,76 @@
         <v>0.104994903160041</v>
       </c>
       <c r="V10">
-        <v>0.1006201155283726</v>
+        <v>0.1025515586726871</v>
       </c>
       <c r="W10">
-        <v>0.09624532789670424</v>
+        <v>0.1001082141853331</v>
       </c>
       <c r="X10">
-        <v>0.09187054026503587</v>
+        <v>0.09766486969797918</v>
       </c>
       <c r="Y10">
-        <v>0.08749575263336749</v>
+        <v>0.09522152521062524</v>
       </c>
       <c r="Z10">
-        <v>0.08312096500169912</v>
+        <v>0.09277818072327131</v>
       </c>
       <c r="AA10">
-        <v>0.07874617737003074</v>
+        <v>0.09033483623591736</v>
       </c>
       <c r="AB10">
-        <v>0.07437138973836237</v>
+        <v>0.08789149174856342</v>
       </c>
       <c r="AC10">
-        <v>0.06999660210669401</v>
+        <v>0.0854481472612095</v>
       </c>
       <c r="AD10">
-        <v>0.06562181447502562</v>
+        <v>0.08300480277385555</v>
       </c>
       <c r="AE10">
-        <v>0.06124702684335724</v>
+        <v>0.0805614582865016</v>
       </c>
       <c r="AF10">
-        <v>0.05687223921168888</v>
+        <v>0.07811811379914768</v>
       </c>
       <c r="AG10">
-        <v>0.0524974515800205</v>
+        <v>0.07567476931179373</v>
       </c>
       <c r="AH10">
-        <v>0.04812266394835213</v>
+        <v>0.0732314248244398</v>
       </c>
       <c r="AI10">
-        <v>0.04374787631668375</v>
+        <v>0.07078808033708586</v>
       </c>
       <c r="AJ10">
-        <v>0.03937308868501537</v>
+        <v>0.06834473584973191</v>
       </c>
       <c r="AK10">
-        <v>0.034998301053347</v>
+        <v>0.06590139136237799</v>
       </c>
       <c r="AL10">
-        <v>0.03062351342167862</v>
+        <v>0.06345804687502404</v>
       </c>
       <c r="AM10">
-        <v>0.02624872579001025</v>
+        <v>0.06101470238767011</v>
       </c>
       <c r="AN10">
-        <v>0.02187393815834188</v>
+        <v>0.05857135790031617</v>
       </c>
       <c r="AO10">
-        <v>0.01749915052667349</v>
+        <v>0.05612801341296222</v>
       </c>
       <c r="AP10">
-        <v>0.01312436289500512</v>
+        <v>0.0536846689256083</v>
       </c>
       <c r="AQ10">
-        <v>0.008749575263336754</v>
+        <v>0.05124132443825435</v>
       </c>
       <c r="AR10">
-        <v>0.004374787631668371</v>
+        <v>0.04879797995090041</v>
       </c>
       <c r="AS10">
-        <v>0</v>
+        <v>0.04635463546354648</v>
       </c>
     </row>
     <row r="11" spans="1:45">
@@ -32446,76 +32446,76 @@
         <v>0.121508664627931</v>
       </c>
       <c r="V11">
-        <v>0.1164458036017672</v>
+        <v>0.1186810271241195</v>
       </c>
       <c r="W11">
-        <v>0.1113829425756034</v>
+        <v>0.1158533896203079</v>
       </c>
       <c r="X11">
-        <v>0.1063200815494396</v>
+        <v>0.1130257521164964</v>
       </c>
       <c r="Y11">
-        <v>0.1012572205232758</v>
+        <v>0.1101981146126848</v>
       </c>
       <c r="Z11">
-        <v>0.09619435949711204</v>
+        <v>0.1073704771088732</v>
       </c>
       <c r="AA11">
-        <v>0.09113149847094826</v>
+        <v>0.1045428396050617</v>
       </c>
       <c r="AB11">
-        <v>0.08606863744478445</v>
+        <v>0.1017152021012502</v>
       </c>
       <c r="AC11">
-        <v>0.08100577641862068</v>
+        <v>0.09888756459743862</v>
       </c>
       <c r="AD11">
-        <v>0.07594291539245687</v>
+        <v>0.09605992709362705</v>
       </c>
       <c r="AE11">
-        <v>0.07088005436629308</v>
+        <v>0.0932322895898155</v>
       </c>
       <c r="AF11">
-        <v>0.0658171933401293</v>
+        <v>0.09040465208600396</v>
       </c>
       <c r="AG11">
-        <v>0.0607543323139655</v>
+        <v>0.08757701458219241</v>
       </c>
       <c r="AH11">
-        <v>0.05569147128780171</v>
+        <v>0.08474937707838086</v>
       </c>
       <c r="AI11">
-        <v>0.05062861026163791</v>
+        <v>0.0819217395745693</v>
       </c>
       <c r="AJ11">
-        <v>0.04556574923547413</v>
+        <v>0.07909410207075776</v>
       </c>
       <c r="AK11">
-        <v>0.04050288820931034</v>
+        <v>0.07626646456694622</v>
       </c>
       <c r="AL11">
-        <v>0.03544002718314654</v>
+        <v>0.07343882706313466</v>
       </c>
       <c r="AM11">
-        <v>0.03037716615698275</v>
+        <v>0.07061118955932311</v>
       </c>
       <c r="AN11">
-        <v>0.02531430513081896</v>
+        <v>0.06778355205551156</v>
       </c>
       <c r="AO11">
-        <v>0.02025144410465516</v>
+        <v>0.06495591455170001</v>
       </c>
       <c r="AP11">
-        <v>0.01518858307849138</v>
+        <v>0.06212827704788847</v>
       </c>
       <c r="AQ11">
-        <v>0.01012572205232759</v>
+        <v>0.05930063954407692</v>
       </c>
       <c r="AR11">
-        <v>0.005062861026163787</v>
+        <v>0.05647300204026537</v>
       </c>
       <c r="AS11">
-        <v>0</v>
+        <v>0.05364536453645382</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -32571,76 +32571,76 @@
         <v>0.0012085881753312</v>
       </c>
       <c r="V12">
-        <v>0.0011582303346924</v>
+        <v>0.001180345026121924</v>
       </c>
       <c r="W12">
-        <v>0.0011078724940536</v>
+        <v>0.001152101876912647</v>
       </c>
       <c r="X12">
-        <v>0.0010575146534148</v>
+        <v>0.001123858727703371</v>
       </c>
       <c r="Y12">
-        <v>0.001007156812776</v>
+        <v>0.001095615578494095</v>
       </c>
       <c r="Z12">
-        <v>0.0009567989721372001</v>
+        <v>0.001067372429284818</v>
       </c>
       <c r="AA12">
-        <v>0.0009064411314984001</v>
+        <v>0.001039129280075542</v>
       </c>
       <c r="AB12">
-        <v>0.0008560832908596</v>
+        <v>0.001010886130866266</v>
       </c>
       <c r="AC12">
-        <v>0.0008057254502208002</v>
+        <v>0.0009826429816569894</v>
       </c>
       <c r="AD12">
-        <v>0.0007553676095820001</v>
+        <v>0.000954399832447713</v>
       </c>
       <c r="AE12">
-        <v>0.0007050097689432</v>
+        <v>0.0009261566832384366</v>
       </c>
       <c r="AF12">
-        <v>0.0006546519283044002</v>
+        <v>0.0008979135340291604</v>
       </c>
       <c r="AG12">
-        <v>0.0006042940876656001</v>
+        <v>0.000869670384819884</v>
       </c>
       <c r="AH12">
-        <v>0.0005539362470268</v>
+        <v>0.0008414272356106076</v>
       </c>
       <c r="AI12">
-        <v>0.000503578406388</v>
+        <v>0.0008131840864013312</v>
       </c>
       <c r="AJ12">
-        <v>0.0004532205657492</v>
+        <v>0.0007849409371920549</v>
       </c>
       <c r="AK12">
-        <v>0.0004028627251104001</v>
+        <v>0.0007566977879827786</v>
       </c>
       <c r="AL12">
-        <v>0.0003525048844716</v>
+        <v>0.0007284546387735021</v>
       </c>
       <c r="AM12">
-        <v>0.0003021470438328</v>
+        <v>0.0007002114895642258</v>
       </c>
       <c r="AN12">
-        <v>0.0002517892031940001</v>
+        <v>0.0006719683403549495</v>
       </c>
       <c r="AO12">
-        <v>0.0002014313625552</v>
+        <v>0.0006437251911456731</v>
       </c>
       <c r="AP12">
-        <v>0.0001510735219164</v>
+        <v>0.0006154820419363967</v>
       </c>
       <c r="AQ12">
-        <v>0.0001007156812776</v>
+        <v>0.0005872388927271204</v>
       </c>
       <c r="AR12">
-        <v>5.035784063879996E-05</v>
+        <v>0.0005589957435178441</v>
       </c>
       <c r="AS12">
-        <v>0</v>
+        <v>0.0005307525943085677</v>
       </c>
     </row>
     <row r="13" spans="1:45">
@@ -32696,76 +32696,76 @@
         <v>0.0012085881753312</v>
       </c>
       <c r="V13">
-        <v>0.03449156366802573</v>
+        <v>0.02199156366802573</v>
       </c>
       <c r="W13">
-        <v>0.06777453916072027</v>
+        <v>0.04277453916072026</v>
       </c>
       <c r="X13">
-        <v>0.1010575146534148</v>
+        <v>0.0635575146534148</v>
       </c>
       <c r="Y13">
-        <v>0.1343404901461093</v>
+        <v>0.08434049014610932</v>
       </c>
       <c r="Z13">
-        <v>0.1676234656388039</v>
+        <v>0.1051234656388039</v>
       </c>
       <c r="AA13">
-        <v>0.2009064411314984</v>
+        <v>0.1259064411314984</v>
       </c>
       <c r="AB13">
-        <v>0.234189416624193</v>
+        <v>0.1466894166241929</v>
       </c>
       <c r="AC13">
-        <v>0.2674723921168874</v>
+        <v>0.1674723921168875</v>
       </c>
       <c r="AD13">
-        <v>0.300755367609582</v>
+        <v>0.188255367609582</v>
       </c>
       <c r="AE13">
-        <v>0.3340383431022766</v>
+        <v>0.2090383431022765</v>
       </c>
       <c r="AF13">
-        <v>0.3673213185949711</v>
+        <v>0.2298213185949711</v>
       </c>
       <c r="AG13">
-        <v>0.4006042940876656</v>
+        <v>0.2506042940876656</v>
       </c>
       <c r="AH13">
-        <v>0.4338872695803602</v>
+        <v>0.2713872695803601</v>
       </c>
       <c r="AI13">
-        <v>0.4671702450730547</v>
+        <v>0.2921702450730547</v>
       </c>
       <c r="AJ13">
-        <v>0.5004532205657491</v>
+        <v>0.3129532205657492</v>
       </c>
       <c r="AK13">
-        <v>0.5337361960584437</v>
+        <v>0.3337361960584437</v>
       </c>
       <c r="AL13">
-        <v>0.5670191715511383</v>
+        <v>0.3545191715511383</v>
       </c>
       <c r="AM13">
-        <v>0.6003021470438329</v>
+        <v>0.3753021470438328</v>
       </c>
       <c r="AN13">
-        <v>0.6335851225365273</v>
+        <v>0.3960851225365273</v>
       </c>
       <c r="AO13">
-        <v>0.666868098029222</v>
+        <v>0.4168680980292219</v>
       </c>
       <c r="AP13">
-        <v>0.7001510735219164</v>
+        <v>0.4376510735219164</v>
       </c>
       <c r="AQ13">
-        <v>0.733434049014611</v>
+        <v>0.4584340490146109</v>
       </c>
       <c r="AR13">
-        <v>0.7667170245073055</v>
+        <v>0.4792170245073055</v>
       </c>
       <c r="AS13">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -32821,76 +32821,76 @@
         <v>0.385539627930683</v>
       </c>
       <c r="V14">
-        <v>0.3736421434335712</v>
+        <v>0.3778088101002379</v>
       </c>
       <c r="W14">
-        <v>0.3617446589364595</v>
+        <v>0.3700779922697928</v>
       </c>
       <c r="X14">
-        <v>0.3498471744393477</v>
+        <v>0.3623471744393477</v>
       </c>
       <c r="Y14">
-        <v>0.3379496899422358</v>
+        <v>0.3546163566089025</v>
       </c>
       <c r="Z14">
-        <v>0.326052205445124</v>
+        <v>0.3468855387784574</v>
       </c>
       <c r="AA14">
-        <v>0.3141547209480123</v>
+        <v>0.3391547209480122</v>
       </c>
       <c r="AB14">
-        <v>0.3022572364509005</v>
+        <v>0.3314239031175671</v>
       </c>
       <c r="AC14">
-        <v>0.2903597519537887</v>
+        <v>0.323693085287122</v>
       </c>
       <c r="AD14">
-        <v>0.2784622674566769</v>
+        <v>0.3159622674566769</v>
       </c>
       <c r="AE14">
-        <v>0.2665647829595651</v>
+        <v>0.3082314496262317</v>
       </c>
       <c r="AF14">
-        <v>0.2546672984624533</v>
+        <v>0.3005006317957867</v>
       </c>
       <c r="AG14">
-        <v>0.2427698139653415</v>
+        <v>0.2927698139653415</v>
       </c>
       <c r="AH14">
-        <v>0.2308723294682297</v>
+        <v>0.2850389961348964</v>
       </c>
       <c r="AI14">
-        <v>0.2189748449711179</v>
+        <v>0.2773081783044513</v>
       </c>
       <c r="AJ14">
-        <v>0.2070773604740061</v>
+        <v>0.2695773604740062</v>
       </c>
       <c r="AK14">
-        <v>0.1951798759768943</v>
+        <v>0.261846542643561</v>
       </c>
       <c r="AL14">
-        <v>0.1832823914797825</v>
+        <v>0.2541157248131159</v>
       </c>
       <c r="AM14">
-        <v>0.1713849069826708</v>
+        <v>0.2463849069826708</v>
       </c>
       <c r="AN14">
-        <v>0.159487422485559</v>
+        <v>0.2386540891522256</v>
       </c>
       <c r="AO14">
-        <v>0.1475899379884472</v>
+        <v>0.2309232713217805</v>
       </c>
       <c r="AP14">
-        <v>0.1356924534913354</v>
+        <v>0.2231924534913354</v>
       </c>
       <c r="AQ14">
-        <v>0.1237949689942236</v>
+        <v>0.2154616356608903</v>
       </c>
       <c r="AR14">
-        <v>0.1118974844971118</v>
+        <v>0.2077308178304451</v>
       </c>
       <c r="AS14">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="1:45">
@@ -32946,76 +32946,76 @@
         <v>0.385539627930683</v>
       </c>
       <c r="V15">
-        <v>0.3736421434335712</v>
+        <v>0.3778088101002379</v>
       </c>
       <c r="W15">
-        <v>0.3617446589364595</v>
+        <v>0.3700779922697928</v>
       </c>
       <c r="X15">
-        <v>0.3498471744393477</v>
+        <v>0.3623471744393477</v>
       </c>
       <c r="Y15">
-        <v>0.3379496899422358</v>
+        <v>0.3546163566089025</v>
       </c>
       <c r="Z15">
-        <v>0.326052205445124</v>
+        <v>0.3468855387784574</v>
       </c>
       <c r="AA15">
-        <v>0.3141547209480123</v>
+        <v>0.3391547209480122</v>
       </c>
       <c r="AB15">
-        <v>0.3022572364509005</v>
+        <v>0.3314239031175671</v>
       </c>
       <c r="AC15">
-        <v>0.2903597519537887</v>
+        <v>0.323693085287122</v>
       </c>
       <c r="AD15">
-        <v>0.2784622674566769</v>
+        <v>0.3159622674566769</v>
       </c>
       <c r="AE15">
-        <v>0.2665647829595651</v>
+        <v>0.3082314496262317</v>
       </c>
       <c r="AF15">
-        <v>0.2546672984624533</v>
+        <v>0.3005006317957867</v>
       </c>
       <c r="AG15">
-        <v>0.2427698139653415</v>
+        <v>0.2927698139653415</v>
       </c>
       <c r="AH15">
-        <v>0.2308723294682297</v>
+        <v>0.2850389961348964</v>
       </c>
       <c r="AI15">
-        <v>0.2189748449711179</v>
+        <v>0.2773081783044513</v>
       </c>
       <c r="AJ15">
-        <v>0.2070773604740061</v>
+        <v>0.2695773604740062</v>
       </c>
       <c r="AK15">
-        <v>0.1951798759768943</v>
+        <v>0.261846542643561</v>
       </c>
       <c r="AL15">
-        <v>0.1832823914797825</v>
+        <v>0.2541157248131159</v>
       </c>
       <c r="AM15">
-        <v>0.1713849069826708</v>
+        <v>0.2463849069826708</v>
       </c>
       <c r="AN15">
-        <v>0.159487422485559</v>
+        <v>0.2386540891522256</v>
       </c>
       <c r="AO15">
-        <v>0.1475899379884472</v>
+        <v>0.2309232713217805</v>
       </c>
       <c r="AP15">
-        <v>0.1356924534913354</v>
+        <v>0.2231924534913354</v>
       </c>
       <c r="AQ15">
-        <v>0.1237949689942236</v>
+        <v>0.2154616356608903</v>
       </c>
       <c r="AR15">
-        <v>0.1118974844971118</v>
+        <v>0.2077308178304451</v>
       </c>
       <c r="AS15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:45">
@@ -33071,76 +33071,76 @@
         <v>0.104994903160041</v>
       </c>
       <c r="V16">
-        <v>0.1006201155283726</v>
+        <v>0.102541307488091</v>
       </c>
       <c r="W16">
-        <v>0.09624532789670424</v>
+        <v>0.100087711816141</v>
       </c>
       <c r="X16">
-        <v>0.09187054026503587</v>
+        <v>0.09763411614419104</v>
       </c>
       <c r="Y16">
-        <v>0.08749575263336749</v>
+        <v>0.09518052047224107</v>
       </c>
       <c r="Z16">
-        <v>0.08312096500169912</v>
+        <v>0.09272692480029109</v>
       </c>
       <c r="AA16">
-        <v>0.07874617737003074</v>
+        <v>0.0902733291283411</v>
       </c>
       <c r="AB16">
-        <v>0.07437138973836237</v>
+        <v>0.08781973345639112</v>
       </c>
       <c r="AC16">
-        <v>0.06999660210669401</v>
+        <v>0.08536613778444115</v>
       </c>
       <c r="AD16">
-        <v>0.06562181447502562</v>
+        <v>0.08291254211249115</v>
       </c>
       <c r="AE16">
-        <v>0.06124702684335724</v>
+        <v>0.08045894644054116</v>
       </c>
       <c r="AF16">
-        <v>0.05687223921168888</v>
+        <v>0.07800535076859119</v>
       </c>
       <c r="AG16">
-        <v>0.0524974515800205</v>
+        <v>0.07555175509664121</v>
       </c>
       <c r="AH16">
-        <v>0.04812266394835213</v>
+        <v>0.07309815942469124</v>
       </c>
       <c r="AI16">
-        <v>0.04374787631668375</v>
+        <v>0.07064456375274125</v>
       </c>
       <c r="AJ16">
-        <v>0.03937308868501537</v>
+        <v>0.06819096808079127</v>
       </c>
       <c r="AK16">
-        <v>0.034998301053347</v>
+        <v>0.06573737240884128</v>
       </c>
       <c r="AL16">
-        <v>0.03062351342167862</v>
+        <v>0.0632837767368913</v>
       </c>
       <c r="AM16">
-        <v>0.02624872579001025</v>
+        <v>0.06083018106494131</v>
       </c>
       <c r="AN16">
-        <v>0.02187393815834188</v>
+        <v>0.05837658539299134</v>
       </c>
       <c r="AO16">
-        <v>0.01749915052667349</v>
+        <v>0.05592298972104135</v>
       </c>
       <c r="AP16">
-        <v>0.01312436289500512</v>
+        <v>0.05346939404909137</v>
       </c>
       <c r="AQ16">
-        <v>0.008749575263336754</v>
+        <v>0.05101579837714139</v>
       </c>
       <c r="AR16">
-        <v>0.004374787631668371</v>
+        <v>0.0485622027051914</v>
       </c>
       <c r="AS16">
-        <v>0</v>
+        <v>0.04610860703324143</v>
       </c>
     </row>
     <row r="17" spans="1:45">
@@ -33196,76 +33196,76 @@
         <v>0.121508664627931</v>
       </c>
       <c r="V17">
-        <v>0.1164458036017672</v>
+        <v>0.118669163617286</v>
       </c>
       <c r="W17">
-        <v>0.1113829425756034</v>
+        <v>0.1158296626066409</v>
       </c>
       <c r="X17">
-        <v>0.1063200815494396</v>
+        <v>0.1129901615959959</v>
       </c>
       <c r="Y17">
-        <v>0.1012572205232758</v>
+        <v>0.1101506605853509</v>
       </c>
       <c r="Z17">
-        <v>0.09619435949711204</v>
+        <v>0.1073111595747059</v>
       </c>
       <c r="AA17">
-        <v>0.09113149847094826</v>
+        <v>0.1044716585640608</v>
       </c>
       <c r="AB17">
-        <v>0.08606863744478445</v>
+        <v>0.1016321575534158</v>
       </c>
       <c r="AC17">
-        <v>0.08100577641862068</v>
+        <v>0.09879265654277078</v>
       </c>
       <c r="AD17">
-        <v>0.07594291539245687</v>
+        <v>0.09595315553212573</v>
       </c>
       <c r="AE17">
-        <v>0.07088005436629308</v>
+        <v>0.0931136545214807</v>
       </c>
       <c r="AF17">
-        <v>0.0658171933401293</v>
+        <v>0.09027415351083568</v>
       </c>
       <c r="AG17">
-        <v>0.0607543323139655</v>
+        <v>0.08743465250019064</v>
       </c>
       <c r="AH17">
-        <v>0.05569147128780171</v>
+        <v>0.08459515148954562</v>
       </c>
       <c r="AI17">
-        <v>0.05062861026163791</v>
+        <v>0.08175565047890059</v>
       </c>
       <c r="AJ17">
-        <v>0.04556574923547413</v>
+        <v>0.07891614946825556</v>
       </c>
       <c r="AK17">
-        <v>0.04050288820931034</v>
+        <v>0.07607664845761053</v>
       </c>
       <c r="AL17">
-        <v>0.03544002718314654</v>
+        <v>0.07323714744696549</v>
       </c>
       <c r="AM17">
-        <v>0.03037716615698275</v>
+        <v>0.07039764643632046</v>
       </c>
       <c r="AN17">
-        <v>0.02531430513081896</v>
+        <v>0.06755814542567544</v>
       </c>
       <c r="AO17">
-        <v>0.02025144410465516</v>
+        <v>0.0647186444150304</v>
       </c>
       <c r="AP17">
-        <v>0.01518858307849138</v>
+        <v>0.06187914340438538</v>
       </c>
       <c r="AQ17">
-        <v>0.01012572205232759</v>
+        <v>0.05903964239374036</v>
       </c>
       <c r="AR17">
-        <v>0.005062861026163787</v>
+        <v>0.05620014138309532</v>
       </c>
       <c r="AS17">
-        <v>0</v>
+        <v>0.05336064037245029</v>
       </c>
     </row>
     <row r="18" spans="1:45">

</xml_diff>

<commit_message>
updated with data from Edmundo from Sunday Nov 3 2024
</commit_message>
<xml_diff>
--- a/iran/transformations/templates/calibrated/iran/model_input_variables_iran_ce_calibrated.xlsx
+++ b/iran/transformations/templates/calibrated/iran/model_input_variables_iran_ce_calibrated.xlsx
@@ -17963,112 +17963,112 @@
         <v>1</v>
       </c>
       <c r="J138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="K138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="L138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="M138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="N138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="O138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="P138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="Q138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="R138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="S138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="T138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="U138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="V138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="W138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="X138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="Y138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="Z138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AA138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AB138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AC138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AD138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AE138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AF138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AG138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AH138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AI138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AJ138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AK138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AL138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AM138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AN138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AO138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AP138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AQ138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AR138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="AS138">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
     </row>
     <row r="139" spans="1:45">
@@ -18088,112 +18088,112 @@
         <v>1</v>
       </c>
       <c r="J139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="K139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="L139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="M139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="N139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="O139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="P139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="Q139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="R139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="S139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="T139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="U139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="V139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="W139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="X139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="Y139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="Z139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AA139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AB139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AC139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AD139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AE139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AF139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AG139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AH139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AI139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AJ139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AK139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AL139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AM139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AN139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AO139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AP139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AQ139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AR139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="AS139">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
     </row>
     <row r="140" spans="1:45">
@@ -34535,70 +34535,70 @@
         <v>1</v>
       </c>
       <c r="J28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="K28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="L28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="M28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="N28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="O28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="P28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="Q28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="R28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="S28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="T28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="U28">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="V28">
-        <v>0.1577669902912621</v>
+        <v>0.1577669902912623</v>
       </c>
       <c r="W28">
-        <v>0.1941747572815533</v>
+        <v>0.1941747572815535</v>
       </c>
       <c r="X28">
-        <v>0.2305825242718446</v>
+        <v>0.2305825242718448</v>
       </c>
       <c r="Y28">
-        <v>0.2669902912621359</v>
+        <v>0.266990291262136</v>
       </c>
       <c r="Z28">
-        <v>0.3033980582524272</v>
+        <v>0.3033980582524273</v>
       </c>
       <c r="AA28">
-        <v>0.3398058252427184</v>
+        <v>0.3398058252427185</v>
       </c>
       <c r="AB28">
-        <v>0.3762135922330097</v>
+        <v>0.3762135922330098</v>
       </c>
       <c r="AC28">
         <v>0.412621359223301</v>
       </c>
       <c r="AD28">
-        <v>0.4490291262135921</v>
+        <v>0.4490291262135923</v>
       </c>
       <c r="AE28">
-        <v>0.4854368932038834</v>
+        <v>0.4854368932038835</v>
       </c>
       <c r="AF28">
         <v>0.5218446601941747</v>
@@ -34610,37 +34610,37 @@
         <v>0.5946601941747572</v>
       </c>
       <c r="AI28">
-        <v>0.6310679611650486</v>
+        <v>0.6310679611650485</v>
       </c>
       <c r="AJ28">
-        <v>0.6674757281553398</v>
+        <v>0.6674757281553397</v>
       </c>
       <c r="AK28">
-        <v>0.7038834951456311</v>
+        <v>0.703883495145631</v>
       </c>
       <c r="AL28">
         <v>0.7402912621359223</v>
       </c>
       <c r="AM28">
-        <v>0.7766990291262135</v>
+        <v>0.7766990291262136</v>
       </c>
       <c r="AN28">
-        <v>0.8131067961165047</v>
+        <v>0.8131067961165048</v>
       </c>
       <c r="AO28">
         <v>0.8495145631067961</v>
       </c>
       <c r="AP28">
-        <v>0.8859223300970873</v>
+        <v>0.8859223300970872</v>
       </c>
       <c r="AQ28">
-        <v>0.9223300970873786</v>
+        <v>0.9223300970873785</v>
       </c>
       <c r="AR28">
-        <v>0.9587378640776699</v>
+        <v>0.9587378640776698</v>
       </c>
       <c r="AS28">
-        <v>0.9951456310679612</v>
+        <v>0.9951456310679611</v>
       </c>
     </row>
     <row r="29" spans="1:45">
@@ -34660,94 +34660,94 @@
         <v>1</v>
       </c>
       <c r="J29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="K29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="L29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="M29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="N29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="O29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="P29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="Q29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="R29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="S29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="T29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="U29">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="V29">
-        <v>0.8373786407766991</v>
+        <v>0.8373786407766988</v>
       </c>
       <c r="W29">
-        <v>0.8009708737864077</v>
+        <v>0.8009708737864075</v>
       </c>
       <c r="X29">
-        <v>0.7645631067961165</v>
+        <v>0.7645631067961163</v>
       </c>
       <c r="Y29">
-        <v>0.7281553398058254</v>
+        <v>0.728155339805825</v>
       </c>
       <c r="Z29">
-        <v>0.691747572815534</v>
+        <v>0.6917475728155338</v>
       </c>
       <c r="AA29">
-        <v>0.6553398058252428</v>
+        <v>0.6553398058252425</v>
       </c>
       <c r="AB29">
-        <v>0.6189320388349514</v>
+        <v>0.6189320388349512</v>
       </c>
       <c r="AC29">
-        <v>0.5825242718446603</v>
+        <v>0.58252427184466</v>
       </c>
       <c r="AD29">
-        <v>0.546116504854369</v>
+        <v>0.5461165048543688</v>
       </c>
       <c r="AE29">
-        <v>0.5097087378640777</v>
+        <v>0.5097087378640774</v>
       </c>
       <c r="AF29">
-        <v>0.4733009708737865</v>
+        <v>0.4733009708737863</v>
       </c>
       <c r="AG29">
-        <v>0.4368932038834952</v>
+        <v>0.436893203883495</v>
       </c>
       <c r="AH29">
-        <v>0.4004854368932039</v>
+        <v>0.4004854368932038</v>
       </c>
       <c r="AI29">
-        <v>0.3640776699029126</v>
+        <v>0.3640776699029125</v>
       </c>
       <c r="AJ29">
-        <v>0.3276699029126214</v>
+        <v>0.3276699029126213</v>
       </c>
       <c r="AK29">
-        <v>0.2912621359223301</v>
+        <v>0.29126213592233</v>
       </c>
       <c r="AL29">
-        <v>0.2548543689320388</v>
+        <v>0.2548543689320387</v>
       </c>
       <c r="AM29">
-        <v>0.2184466019417476</v>
+        <v>0.2184466019417475</v>
       </c>
       <c r="AN29">
         <v>0.1820388349514563</v>
@@ -34759,10 +34759,10 @@
         <v>0.1092233009708738</v>
       </c>
       <c r="AQ29">
-        <v>0.07281553398058256</v>
+        <v>0.07281553398058253</v>
       </c>
       <c r="AR29">
-        <v>0.03640776699029123</v>
+        <v>0.03640776699029122</v>
       </c>
       <c r="AS29">
         <v>0</v>
@@ -39929,70 +39929,70 @@
         <v>1</v>
       </c>
       <c r="J29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="K29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="L29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="M29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="N29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="O29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="P29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="Q29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="R29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="S29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="T29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="U29">
-        <v>0.1213592233009708</v>
+        <v>0.121359223300971</v>
       </c>
       <c r="V29">
-        <v>0.1577669902912621</v>
+        <v>0.1577669902912623</v>
       </c>
       <c r="W29">
-        <v>0.1941747572815533</v>
+        <v>0.1941747572815535</v>
       </c>
       <c r="X29">
-        <v>0.2305825242718446</v>
+        <v>0.2305825242718448</v>
       </c>
       <c r="Y29">
-        <v>0.2669902912621359</v>
+        <v>0.266990291262136</v>
       </c>
       <c r="Z29">
-        <v>0.3033980582524272</v>
+        <v>0.3033980582524273</v>
       </c>
       <c r="AA29">
-        <v>0.3398058252427184</v>
+        <v>0.3398058252427185</v>
       </c>
       <c r="AB29">
-        <v>0.3762135922330097</v>
+        <v>0.3762135922330098</v>
       </c>
       <c r="AC29">
         <v>0.412621359223301</v>
       </c>
       <c r="AD29">
-        <v>0.4490291262135921</v>
+        <v>0.4490291262135923</v>
       </c>
       <c r="AE29">
-        <v>0.4854368932038834</v>
+        <v>0.4854368932038835</v>
       </c>
       <c r="AF29">
         <v>0.5218446601941747</v>
@@ -40004,37 +40004,37 @@
         <v>0.5946601941747572</v>
       </c>
       <c r="AI29">
-        <v>0.6310679611650486</v>
+        <v>0.6310679611650485</v>
       </c>
       <c r="AJ29">
-        <v>0.6674757281553398</v>
+        <v>0.6674757281553397</v>
       </c>
       <c r="AK29">
-        <v>0.7038834951456311</v>
+        <v>0.703883495145631</v>
       </c>
       <c r="AL29">
         <v>0.7402912621359223</v>
       </c>
       <c r="AM29">
-        <v>0.7766990291262135</v>
+        <v>0.7766990291262136</v>
       </c>
       <c r="AN29">
-        <v>0.8131067961165047</v>
+        <v>0.8131067961165048</v>
       </c>
       <c r="AO29">
         <v>0.8495145631067961</v>
       </c>
       <c r="AP29">
-        <v>0.8859223300970873</v>
+        <v>0.8859223300970872</v>
       </c>
       <c r="AQ29">
-        <v>0.9223300970873786</v>
+        <v>0.9223300970873785</v>
       </c>
       <c r="AR29">
-        <v>0.9587378640776699</v>
+        <v>0.9587378640776698</v>
       </c>
       <c r="AS29">
-        <v>0.9951456310679612</v>
+        <v>0.9951456310679611</v>
       </c>
     </row>
     <row r="30" spans="1:45">
@@ -40054,94 +40054,94 @@
         <v>1</v>
       </c>
       <c r="J30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="K30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="L30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="M30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="N30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="O30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="P30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="Q30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="R30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="S30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="T30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="U30">
-        <v>0.8737864077669903</v>
+        <v>0.87378640776699</v>
       </c>
       <c r="V30">
-        <v>0.8373786407766991</v>
+        <v>0.8373786407766988</v>
       </c>
       <c r="W30">
-        <v>0.8009708737864077</v>
+        <v>0.8009708737864075</v>
       </c>
       <c r="X30">
-        <v>0.7645631067961165</v>
+        <v>0.7645631067961163</v>
       </c>
       <c r="Y30">
-        <v>0.7281553398058254</v>
+        <v>0.728155339805825</v>
       </c>
       <c r="Z30">
-        <v>0.691747572815534</v>
+        <v>0.6917475728155338</v>
       </c>
       <c r="AA30">
-        <v>0.6553398058252428</v>
+        <v>0.6553398058252425</v>
       </c>
       <c r="AB30">
-        <v>0.6189320388349514</v>
+        <v>0.6189320388349512</v>
       </c>
       <c r="AC30">
-        <v>0.5825242718446603</v>
+        <v>0.58252427184466</v>
       </c>
       <c r="AD30">
-        <v>0.546116504854369</v>
+        <v>0.5461165048543688</v>
       </c>
       <c r="AE30">
-        <v>0.5097087378640777</v>
+        <v>0.5097087378640774</v>
       </c>
       <c r="AF30">
-        <v>0.4733009708737865</v>
+        <v>0.4733009708737863</v>
       </c>
       <c r="AG30">
-        <v>0.4368932038834952</v>
+        <v>0.436893203883495</v>
       </c>
       <c r="AH30">
-        <v>0.4004854368932039</v>
+        <v>0.4004854368932038</v>
       </c>
       <c r="AI30">
-        <v>0.3640776699029126</v>
+        <v>0.3640776699029125</v>
       </c>
       <c r="AJ30">
-        <v>0.3276699029126214</v>
+        <v>0.3276699029126213</v>
       </c>
       <c r="AK30">
-        <v>0.2912621359223301</v>
+        <v>0.29126213592233</v>
       </c>
       <c r="AL30">
-        <v>0.2548543689320388</v>
+        <v>0.2548543689320387</v>
       </c>
       <c r="AM30">
-        <v>0.2184466019417476</v>
+        <v>0.2184466019417475</v>
       </c>
       <c r="AN30">
         <v>0.1820388349514563</v>
@@ -40153,10 +40153,10 @@
         <v>0.1092233009708738</v>
       </c>
       <c r="AQ30">
-        <v>0.07281553398058256</v>
+        <v>0.07281553398058253</v>
       </c>
       <c r="AR30">
-        <v>0.03640776699029123</v>
+        <v>0.03640776699029122</v>
       </c>
       <c r="AS30">
         <v>0</v>

</xml_diff>

<commit_message>
updated work on Iran
</commit_message>
<xml_diff>
--- a/iran/transformations/templates/calibrated/iran/model_input_variables_iran_ce_calibrated.xlsx
+++ b/iran/transformations/templates/calibrated/iran/model_input_variables_iran_ce_calibrated.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="237">
   <si>
     <t>subsector</t>
   </si>
@@ -28850,7 +28850,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS18"/>
+  <dimension ref="A1:AS25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -31116,6 +31116,881 @@
       </c>
       <c r="AS18">
         <v>0.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:45">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19">
+        <v>23</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0.05</v>
+      </c>
+      <c r="K19">
+        <v>0.05</v>
+      </c>
+      <c r="L19">
+        <v>0.05</v>
+      </c>
+      <c r="M19">
+        <v>0.05</v>
+      </c>
+      <c r="N19">
+        <v>0.05</v>
+      </c>
+      <c r="O19">
+        <v>0.05</v>
+      </c>
+      <c r="P19">
+        <v>0.05</v>
+      </c>
+      <c r="Q19">
+        <v>0.05</v>
+      </c>
+      <c r="R19">
+        <v>0.05</v>
+      </c>
+      <c r="S19">
+        <v>0.05</v>
+      </c>
+      <c r="T19">
+        <v>0.05</v>
+      </c>
+      <c r="U19">
+        <v>0.05</v>
+      </c>
+      <c r="V19">
+        <v>0.06041666666666667</v>
+      </c>
+      <c r="W19">
+        <v>0.07083333333333333</v>
+      </c>
+      <c r="X19">
+        <v>0.08125</v>
+      </c>
+      <c r="Y19">
+        <v>0.09166666666666667</v>
+      </c>
+      <c r="Z19">
+        <v>0.1020833333333333</v>
+      </c>
+      <c r="AA19">
+        <v>0.1125</v>
+      </c>
+      <c r="AB19">
+        <v>0.1229166666666667</v>
+      </c>
+      <c r="AC19">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="AD19">
+        <v>0.14375</v>
+      </c>
+      <c r="AE19">
+        <v>0.1541666666666667</v>
+      </c>
+      <c r="AF19">
+        <v>0.1645833333333333</v>
+      </c>
+      <c r="AG19">
+        <v>0.175</v>
+      </c>
+      <c r="AH19">
+        <v>0.1854166666666666</v>
+      </c>
+      <c r="AI19">
+        <v>0.1958333333333334</v>
+      </c>
+      <c r="AJ19">
+        <v>0.20625</v>
+      </c>
+      <c r="AK19">
+        <v>0.2166666666666666</v>
+      </c>
+      <c r="AL19">
+        <v>0.2270833333333333</v>
+      </c>
+      <c r="AM19">
+        <v>0.2375</v>
+      </c>
+      <c r="AN19">
+        <v>0.2479166666666666</v>
+      </c>
+      <c r="AO19">
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="AP19">
+        <v>0.26875</v>
+      </c>
+      <c r="AQ19">
+        <v>0.2791666666666666</v>
+      </c>
+      <c r="AR19">
+        <v>0.2895833333333333</v>
+      </c>
+      <c r="AS19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:45">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20">
+        <v>23</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0.05</v>
+      </c>
+      <c r="K20">
+        <v>0.05</v>
+      </c>
+      <c r="L20">
+        <v>0.05</v>
+      </c>
+      <c r="M20">
+        <v>0.05</v>
+      </c>
+      <c r="N20">
+        <v>0.05</v>
+      </c>
+      <c r="O20">
+        <v>0.05</v>
+      </c>
+      <c r="P20">
+        <v>0.05</v>
+      </c>
+      <c r="Q20">
+        <v>0.05</v>
+      </c>
+      <c r="R20">
+        <v>0.05</v>
+      </c>
+      <c r="S20">
+        <v>0.05</v>
+      </c>
+      <c r="T20">
+        <v>0.05</v>
+      </c>
+      <c r="U20">
+        <v>0.05</v>
+      </c>
+      <c r="V20">
+        <v>0.06041666666666667</v>
+      </c>
+      <c r="W20">
+        <v>0.07083333333333333</v>
+      </c>
+      <c r="X20">
+        <v>0.08125</v>
+      </c>
+      <c r="Y20">
+        <v>0.09166666666666667</v>
+      </c>
+      <c r="Z20">
+        <v>0.1020833333333333</v>
+      </c>
+      <c r="AA20">
+        <v>0.1125</v>
+      </c>
+      <c r="AB20">
+        <v>0.1229166666666667</v>
+      </c>
+      <c r="AC20">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="AD20">
+        <v>0.14375</v>
+      </c>
+      <c r="AE20">
+        <v>0.1541666666666667</v>
+      </c>
+      <c r="AF20">
+        <v>0.1645833333333333</v>
+      </c>
+      <c r="AG20">
+        <v>0.175</v>
+      </c>
+      <c r="AH20">
+        <v>0.1854166666666666</v>
+      </c>
+      <c r="AI20">
+        <v>0.1958333333333334</v>
+      </c>
+      <c r="AJ20">
+        <v>0.20625</v>
+      </c>
+      <c r="AK20">
+        <v>0.2166666666666666</v>
+      </c>
+      <c r="AL20">
+        <v>0.2270833333333333</v>
+      </c>
+      <c r="AM20">
+        <v>0.2375</v>
+      </c>
+      <c r="AN20">
+        <v>0.2479166666666666</v>
+      </c>
+      <c r="AO20">
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="AP20">
+        <v>0.26875</v>
+      </c>
+      <c r="AQ20">
+        <v>0.2791666666666666</v>
+      </c>
+      <c r="AR20">
+        <v>0.2895833333333333</v>
+      </c>
+      <c r="AS20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:45">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0.05</v>
+      </c>
+      <c r="K21">
+        <v>0.05</v>
+      </c>
+      <c r="L21">
+        <v>0.05</v>
+      </c>
+      <c r="M21">
+        <v>0.05</v>
+      </c>
+      <c r="N21">
+        <v>0.05</v>
+      </c>
+      <c r="O21">
+        <v>0.05</v>
+      </c>
+      <c r="P21">
+        <v>0.05</v>
+      </c>
+      <c r="Q21">
+        <v>0.05</v>
+      </c>
+      <c r="R21">
+        <v>0.05</v>
+      </c>
+      <c r="S21">
+        <v>0.05</v>
+      </c>
+      <c r="T21">
+        <v>0.05</v>
+      </c>
+      <c r="U21">
+        <v>0.05</v>
+      </c>
+      <c r="V21">
+        <v>0.06041666666666667</v>
+      </c>
+      <c r="W21">
+        <v>0.07083333333333333</v>
+      </c>
+      <c r="X21">
+        <v>0.08125</v>
+      </c>
+      <c r="Y21">
+        <v>0.09166666666666667</v>
+      </c>
+      <c r="Z21">
+        <v>0.1020833333333333</v>
+      </c>
+      <c r="AA21">
+        <v>0.1125</v>
+      </c>
+      <c r="AB21">
+        <v>0.1229166666666667</v>
+      </c>
+      <c r="AC21">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="AD21">
+        <v>0.14375</v>
+      </c>
+      <c r="AE21">
+        <v>0.1541666666666667</v>
+      </c>
+      <c r="AF21">
+        <v>0.1645833333333333</v>
+      </c>
+      <c r="AG21">
+        <v>0.175</v>
+      </c>
+      <c r="AH21">
+        <v>0.1854166666666666</v>
+      </c>
+      <c r="AI21">
+        <v>0.1958333333333334</v>
+      </c>
+      <c r="AJ21">
+        <v>0.20625</v>
+      </c>
+      <c r="AK21">
+        <v>0.2166666666666666</v>
+      </c>
+      <c r="AL21">
+        <v>0.2270833333333333</v>
+      </c>
+      <c r="AM21">
+        <v>0.2375</v>
+      </c>
+      <c r="AN21">
+        <v>0.2479166666666666</v>
+      </c>
+      <c r="AO21">
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="AP21">
+        <v>0.26875</v>
+      </c>
+      <c r="AQ21">
+        <v>0.2791666666666666</v>
+      </c>
+      <c r="AR21">
+        <v>0.2895833333333333</v>
+      </c>
+      <c r="AS21">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22">
+        <v>23</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0.05</v>
+      </c>
+      <c r="K22">
+        <v>0.05</v>
+      </c>
+      <c r="L22">
+        <v>0.05</v>
+      </c>
+      <c r="M22">
+        <v>0.05</v>
+      </c>
+      <c r="N22">
+        <v>0.05</v>
+      </c>
+      <c r="O22">
+        <v>0.05</v>
+      </c>
+      <c r="P22">
+        <v>0.05</v>
+      </c>
+      <c r="Q22">
+        <v>0.05</v>
+      </c>
+      <c r="R22">
+        <v>0.05</v>
+      </c>
+      <c r="S22">
+        <v>0.05</v>
+      </c>
+      <c r="T22">
+        <v>0.05</v>
+      </c>
+      <c r="U22">
+        <v>0.05</v>
+      </c>
+      <c r="V22">
+        <v>0.06041666666666667</v>
+      </c>
+      <c r="W22">
+        <v>0.07083333333333333</v>
+      </c>
+      <c r="X22">
+        <v>0.08125</v>
+      </c>
+      <c r="Y22">
+        <v>0.09166666666666667</v>
+      </c>
+      <c r="Z22">
+        <v>0.1020833333333333</v>
+      </c>
+      <c r="AA22">
+        <v>0.1125</v>
+      </c>
+      <c r="AB22">
+        <v>0.1229166666666667</v>
+      </c>
+      <c r="AC22">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="AD22">
+        <v>0.14375</v>
+      </c>
+      <c r="AE22">
+        <v>0.1541666666666667</v>
+      </c>
+      <c r="AF22">
+        <v>0.1645833333333333</v>
+      </c>
+      <c r="AG22">
+        <v>0.175</v>
+      </c>
+      <c r="AH22">
+        <v>0.1854166666666666</v>
+      </c>
+      <c r="AI22">
+        <v>0.1958333333333334</v>
+      </c>
+      <c r="AJ22">
+        <v>0.20625</v>
+      </c>
+      <c r="AK22">
+        <v>0.2166666666666666</v>
+      </c>
+      <c r="AL22">
+        <v>0.2270833333333333</v>
+      </c>
+      <c r="AM22">
+        <v>0.2375</v>
+      </c>
+      <c r="AN22">
+        <v>0.2479166666666666</v>
+      </c>
+      <c r="AO22">
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="AP22">
+        <v>0.26875</v>
+      </c>
+      <c r="AQ22">
+        <v>0.2791666666666666</v>
+      </c>
+      <c r="AR22">
+        <v>0.2895833333333333</v>
+      </c>
+      <c r="AS22">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:45">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0.05</v>
+      </c>
+      <c r="K23">
+        <v>0.05</v>
+      </c>
+      <c r="L23">
+        <v>0.05</v>
+      </c>
+      <c r="M23">
+        <v>0.05</v>
+      </c>
+      <c r="N23">
+        <v>0.05</v>
+      </c>
+      <c r="O23">
+        <v>0.05</v>
+      </c>
+      <c r="P23">
+        <v>0.05</v>
+      </c>
+      <c r="Q23">
+        <v>0.05</v>
+      </c>
+      <c r="R23">
+        <v>0.05</v>
+      </c>
+      <c r="S23">
+        <v>0.05</v>
+      </c>
+      <c r="T23">
+        <v>0.05</v>
+      </c>
+      <c r="U23">
+        <v>0.05</v>
+      </c>
+      <c r="V23">
+        <v>0.06041666666666667</v>
+      </c>
+      <c r="W23">
+        <v>0.07083333333333333</v>
+      </c>
+      <c r="X23">
+        <v>0.08125</v>
+      </c>
+      <c r="Y23">
+        <v>0.09166666666666667</v>
+      </c>
+      <c r="Z23">
+        <v>0.1020833333333333</v>
+      </c>
+      <c r="AA23">
+        <v>0.1125</v>
+      </c>
+      <c r="AB23">
+        <v>0.1229166666666667</v>
+      </c>
+      <c r="AC23">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="AD23">
+        <v>0.14375</v>
+      </c>
+      <c r="AE23">
+        <v>0.1541666666666667</v>
+      </c>
+      <c r="AF23">
+        <v>0.1645833333333333</v>
+      </c>
+      <c r="AG23">
+        <v>0.175</v>
+      </c>
+      <c r="AH23">
+        <v>0.1854166666666666</v>
+      </c>
+      <c r="AI23">
+        <v>0.1958333333333334</v>
+      </c>
+      <c r="AJ23">
+        <v>0.20625</v>
+      </c>
+      <c r="AK23">
+        <v>0.2166666666666666</v>
+      </c>
+      <c r="AL23">
+        <v>0.2270833333333333</v>
+      </c>
+      <c r="AM23">
+        <v>0.2375</v>
+      </c>
+      <c r="AN23">
+        <v>0.2479166666666666</v>
+      </c>
+      <c r="AO23">
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="AP23">
+        <v>0.26875</v>
+      </c>
+      <c r="AQ23">
+        <v>0.2791666666666666</v>
+      </c>
+      <c r="AR23">
+        <v>0.2895833333333333</v>
+      </c>
+      <c r="AS23">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:45">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0.05</v>
+      </c>
+      <c r="K24">
+        <v>0.05</v>
+      </c>
+      <c r="L24">
+        <v>0.05</v>
+      </c>
+      <c r="M24">
+        <v>0.05</v>
+      </c>
+      <c r="N24">
+        <v>0.05</v>
+      </c>
+      <c r="O24">
+        <v>0.05</v>
+      </c>
+      <c r="P24">
+        <v>0.05</v>
+      </c>
+      <c r="Q24">
+        <v>0.05</v>
+      </c>
+      <c r="R24">
+        <v>0.05</v>
+      </c>
+      <c r="S24">
+        <v>0.05</v>
+      </c>
+      <c r="T24">
+        <v>0.05</v>
+      </c>
+      <c r="U24">
+        <v>0.05</v>
+      </c>
+      <c r="V24">
+        <v>0.06041666666666667</v>
+      </c>
+      <c r="W24">
+        <v>0.07083333333333333</v>
+      </c>
+      <c r="X24">
+        <v>0.08125</v>
+      </c>
+      <c r="Y24">
+        <v>0.09166666666666667</v>
+      </c>
+      <c r="Z24">
+        <v>0.1020833333333333</v>
+      </c>
+      <c r="AA24">
+        <v>0.1125</v>
+      </c>
+      <c r="AB24">
+        <v>0.1229166666666667</v>
+      </c>
+      <c r="AC24">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="AD24">
+        <v>0.14375</v>
+      </c>
+      <c r="AE24">
+        <v>0.1541666666666667</v>
+      </c>
+      <c r="AF24">
+        <v>0.1645833333333333</v>
+      </c>
+      <c r="AG24">
+        <v>0.175</v>
+      </c>
+      <c r="AH24">
+        <v>0.1854166666666666</v>
+      </c>
+      <c r="AI24">
+        <v>0.1958333333333334</v>
+      </c>
+      <c r="AJ24">
+        <v>0.20625</v>
+      </c>
+      <c r="AK24">
+        <v>0.2166666666666666</v>
+      </c>
+      <c r="AL24">
+        <v>0.2270833333333333</v>
+      </c>
+      <c r="AM24">
+        <v>0.2375</v>
+      </c>
+      <c r="AN24">
+        <v>0.2479166666666666</v>
+      </c>
+      <c r="AO24">
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="AP24">
+        <v>0.26875</v>
+      </c>
+      <c r="AQ24">
+        <v>0.2791666666666666</v>
+      </c>
+      <c r="AR24">
+        <v>0.2895833333333333</v>
+      </c>
+      <c r="AS24">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:45">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>0.05</v>
+      </c>
+      <c r="K25">
+        <v>0.05</v>
+      </c>
+      <c r="L25">
+        <v>0.05</v>
+      </c>
+      <c r="M25">
+        <v>0.05</v>
+      </c>
+      <c r="N25">
+        <v>0.05</v>
+      </c>
+      <c r="O25">
+        <v>0.05</v>
+      </c>
+      <c r="P25">
+        <v>0.05</v>
+      </c>
+      <c r="Q25">
+        <v>0.05</v>
+      </c>
+      <c r="R25">
+        <v>0.05</v>
+      </c>
+      <c r="S25">
+        <v>0.05</v>
+      </c>
+      <c r="T25">
+        <v>0.05</v>
+      </c>
+      <c r="U25">
+        <v>0.05</v>
+      </c>
+      <c r="V25">
+        <v>0.06041666666666667</v>
+      </c>
+      <c r="W25">
+        <v>0.07083333333333333</v>
+      </c>
+      <c r="X25">
+        <v>0.08125</v>
+      </c>
+      <c r="Y25">
+        <v>0.09166666666666667</v>
+      </c>
+      <c r="Z25">
+        <v>0.1020833333333333</v>
+      </c>
+      <c r="AA25">
+        <v>0.1125</v>
+      </c>
+      <c r="AB25">
+        <v>0.1229166666666667</v>
+      </c>
+      <c r="AC25">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="AD25">
+        <v>0.14375</v>
+      </c>
+      <c r="AE25">
+        <v>0.1541666666666667</v>
+      </c>
+      <c r="AF25">
+        <v>0.1645833333333333</v>
+      </c>
+      <c r="AG25">
+        <v>0.175</v>
+      </c>
+      <c r="AH25">
+        <v>0.1854166666666666</v>
+      </c>
+      <c r="AI25">
+        <v>0.1958333333333334</v>
+      </c>
+      <c r="AJ25">
+        <v>0.20625</v>
+      </c>
+      <c r="AK25">
+        <v>0.2166666666666666</v>
+      </c>
+      <c r="AL25">
+        <v>0.2270833333333333</v>
+      </c>
+      <c r="AM25">
+        <v>0.2375</v>
+      </c>
+      <c r="AN25">
+        <v>0.2479166666666666</v>
+      </c>
+      <c r="AO25">
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="AP25">
+        <v>0.26875</v>
+      </c>
+      <c r="AQ25">
+        <v>0.2791666666666666</v>
+      </c>
+      <c r="AR25">
+        <v>0.2895833333333333</v>
+      </c>
+      <c r="AS25">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -33273,10 +34148,10 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C18">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -33285,112 +34160,112 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="L18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="M18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="N18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="O18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="P18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="Q18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="R18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="S18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="T18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="U18">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="V18">
-        <v>0.03895833333333333</v>
+        <v>0.9791666666666667</v>
       </c>
       <c r="W18">
-        <v>0.05791666666666666</v>
+        <v>0.9583333333333333</v>
       </c>
       <c r="X18">
-        <v>0.076875</v>
+        <v>0.9375</v>
       </c>
       <c r="Y18">
-        <v>0.09583333333333333</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="Z18">
-        <v>0.1147916666666667</v>
+        <v>0.8958333333333333</v>
       </c>
       <c r="AA18">
-        <v>0.13375</v>
+        <v>0.875</v>
       </c>
       <c r="AB18">
-        <v>0.1527083333333333</v>
+        <v>0.8541666666666666</v>
       </c>
       <c r="AC18">
-        <v>0.1716666666666667</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AD18">
-        <v>0.190625</v>
+        <v>0.8125</v>
       </c>
       <c r="AE18">
-        <v>0.2095833333333333</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="AF18">
-        <v>0.2285416666666666</v>
+        <v>0.7708333333333334</v>
       </c>
       <c r="AG18">
-        <v>0.2475</v>
+        <v>0.75</v>
       </c>
       <c r="AH18">
-        <v>0.2664583333333333</v>
+        <v>0.7291666666666667</v>
       </c>
       <c r="AI18">
-        <v>0.2854166666666667</v>
+        <v>0.7083333333333333</v>
       </c>
       <c r="AJ18">
-        <v>0.304375</v>
+        <v>0.6875</v>
       </c>
       <c r="AK18">
-        <v>0.3233333333333333</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="AL18">
-        <v>0.3422916666666667</v>
+        <v>0.6458333333333333</v>
       </c>
       <c r="AM18">
-        <v>0.36125</v>
+        <v>0.625</v>
       </c>
       <c r="AN18">
-        <v>0.3802083333333333</v>
+        <v>0.6041666666666667</v>
       </c>
       <c r="AO18">
-        <v>0.3991666666666667</v>
+        <v>0.5833333333333333</v>
       </c>
       <c r="AP18">
-        <v>0.418125</v>
+        <v>0.5625</v>
       </c>
       <c r="AQ18">
-        <v>0.4370833333333333</v>
+        <v>0.5416666666666667</v>
       </c>
       <c r="AR18">
-        <v>0.4560416666666667</v>
+        <v>0.5208333333333333</v>
       </c>
       <c r="AS18">
-        <v>0.475</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:45">
@@ -33398,7 +34273,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C19">
         <v>22</v>
@@ -33410,112 +34285,112 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="K19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="L19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="M19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="N19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="O19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="P19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="Q19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="R19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="S19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="T19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="U19">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="V19">
-        <v>0.403125</v>
+        <v>0.030625</v>
       </c>
       <c r="W19">
-        <v>0.40625</v>
+        <v>0.04125</v>
       </c>
       <c r="X19">
-        <v>0.409375</v>
+        <v>0.051875</v>
       </c>
       <c r="Y19">
-        <v>0.4125</v>
+        <v>0.0625</v>
       </c>
       <c r="Z19">
-        <v>0.415625</v>
+        <v>0.073125</v>
       </c>
       <c r="AA19">
-        <v>0.4187500000000001</v>
+        <v>0.08375</v>
       </c>
       <c r="AB19">
-        <v>0.421875</v>
+        <v>0.094375</v>
       </c>
       <c r="AC19">
-        <v>0.425</v>
+        <v>0.105</v>
       </c>
       <c r="AD19">
-        <v>0.428125</v>
+        <v>0.115625</v>
       </c>
       <c r="AE19">
-        <v>0.43125</v>
+        <v>0.12625</v>
       </c>
       <c r="AF19">
-        <v>0.434375</v>
+        <v>0.136875</v>
       </c>
       <c r="AG19">
-        <v>0.4375</v>
+        <v>0.1475</v>
       </c>
       <c r="AH19">
-        <v>0.440625</v>
+        <v>0.158125</v>
       </c>
       <c r="AI19">
-        <v>0.44375</v>
+        <v>0.16875</v>
       </c>
       <c r="AJ19">
-        <v>0.446875</v>
+        <v>0.179375</v>
       </c>
       <c r="AK19">
-        <v>0.45</v>
+        <v>0.19</v>
       </c>
       <c r="AL19">
-        <v>0.453125</v>
+        <v>0.200625</v>
       </c>
       <c r="AM19">
-        <v>0.4562499999999999</v>
+        <v>0.21125</v>
       </c>
       <c r="AN19">
-        <v>0.459375</v>
+        <v>0.221875</v>
       </c>
       <c r="AO19">
-        <v>0.4625</v>
+        <v>0.2325</v>
       </c>
       <c r="AP19">
-        <v>0.465625</v>
+        <v>0.243125</v>
       </c>
       <c r="AQ19">
-        <v>0.4687499999999999</v>
+        <v>0.25375</v>
       </c>
       <c r="AR19">
-        <v>0.471875</v>
+        <v>0.264375</v>
       </c>
       <c r="AS19">
-        <v>0.475</v>
+        <v>0.275</v>
       </c>
     </row>
     <row r="20" spans="1:45">
@@ -33571,76 +34446,76 @@
         <v>0.02</v>
       </c>
       <c r="V20">
-        <v>0.03895833333333333</v>
+        <v>0.030625</v>
       </c>
       <c r="W20">
-        <v>0.05791666666666666</v>
+        <v>0.04125</v>
       </c>
       <c r="X20">
-        <v>0.076875</v>
+        <v>0.051875</v>
       </c>
       <c r="Y20">
-        <v>0.09583333333333333</v>
+        <v>0.0625</v>
       </c>
       <c r="Z20">
-        <v>0.1147916666666667</v>
+        <v>0.073125</v>
       </c>
       <c r="AA20">
-        <v>0.13375</v>
+        <v>0.08375</v>
       </c>
       <c r="AB20">
-        <v>0.1527083333333333</v>
+        <v>0.094375</v>
       </c>
       <c r="AC20">
-        <v>0.1716666666666667</v>
+        <v>0.105</v>
       </c>
       <c r="AD20">
-        <v>0.190625</v>
+        <v>0.115625</v>
       </c>
       <c r="AE20">
-        <v>0.2095833333333333</v>
+        <v>0.12625</v>
       </c>
       <c r="AF20">
-        <v>0.2285416666666666</v>
+        <v>0.136875</v>
       </c>
       <c r="AG20">
-        <v>0.2475</v>
+        <v>0.1475</v>
       </c>
       <c r="AH20">
-        <v>0.2664583333333333</v>
+        <v>0.158125</v>
       </c>
       <c r="AI20">
-        <v>0.2854166666666667</v>
+        <v>0.16875</v>
       </c>
       <c r="AJ20">
-        <v>0.304375</v>
+        <v>0.179375</v>
       </c>
       <c r="AK20">
-        <v>0.3233333333333333</v>
+        <v>0.19</v>
       </c>
       <c r="AL20">
-        <v>0.3422916666666667</v>
+        <v>0.200625</v>
       </c>
       <c r="AM20">
-        <v>0.36125</v>
+        <v>0.21125</v>
       </c>
       <c r="AN20">
-        <v>0.3802083333333333</v>
+        <v>0.221875</v>
       </c>
       <c r="AO20">
-        <v>0.3991666666666667</v>
+        <v>0.2325</v>
       </c>
       <c r="AP20">
-        <v>0.418125</v>
+        <v>0.243125</v>
       </c>
       <c r="AQ20">
-        <v>0.4370833333333333</v>
+        <v>0.25375</v>
       </c>
       <c r="AR20">
-        <v>0.4560416666666667</v>
+        <v>0.264375</v>
       </c>
       <c r="AS20">
-        <v>0.475</v>
+        <v>0.275</v>
       </c>
     </row>
     <row r="21" spans="1:45">
@@ -33696,76 +34571,76 @@
         <v>0.03</v>
       </c>
       <c r="V21">
-        <v>0.04854166666666666</v>
+        <v>0.04020833333333333</v>
       </c>
       <c r="W21">
-        <v>0.06708333333333333</v>
+        <v>0.05041666666666667</v>
       </c>
       <c r="X21">
-        <v>0.08562499999999999</v>
+        <v>0.060625</v>
       </c>
       <c r="Y21">
-        <v>0.1041666666666667</v>
+        <v>0.07083333333333333</v>
       </c>
       <c r="Z21">
-        <v>0.1227083333333333</v>
+        <v>0.08104166666666666</v>
       </c>
       <c r="AA21">
-        <v>0.14125</v>
+        <v>0.09125</v>
       </c>
       <c r="AB21">
-        <v>0.1597916666666667</v>
+        <v>0.1014583333333333</v>
       </c>
       <c r="AC21">
-        <v>0.1783333333333333</v>
+        <v>0.1116666666666667</v>
       </c>
       <c r="AD21">
-        <v>0.196875</v>
+        <v>0.121875</v>
       </c>
       <c r="AE21">
-        <v>0.2154166666666666</v>
+        <v>0.1320833333333333</v>
       </c>
       <c r="AF21">
-        <v>0.2339583333333333</v>
+        <v>0.1422916666666666</v>
       </c>
       <c r="AG21">
-        <v>0.2525</v>
+        <v>0.1525</v>
       </c>
       <c r="AH21">
-        <v>0.2710416666666666</v>
+        <v>0.1627083333333333</v>
       </c>
       <c r="AI21">
-        <v>0.2895833333333334</v>
+        <v>0.1729166666666667</v>
       </c>
       <c r="AJ21">
-        <v>0.308125</v>
+        <v>0.183125</v>
       </c>
       <c r="AK21">
-        <v>0.3266666666666667</v>
+        <v>0.1933333333333334</v>
       </c>
       <c r="AL21">
-        <v>0.3452083333333333</v>
+        <v>0.2035416666666667</v>
       </c>
       <c r="AM21">
-        <v>0.36375</v>
+        <v>0.21375</v>
       </c>
       <c r="AN21">
-        <v>0.3822916666666666</v>
+        <v>0.2239583333333333</v>
       </c>
       <c r="AO21">
-        <v>0.4008333333333333</v>
+        <v>0.2341666666666667</v>
       </c>
       <c r="AP21">
-        <v>0.4193749999999999</v>
+        <v>0.244375</v>
       </c>
       <c r="AQ21">
-        <v>0.4379166666666666</v>
+        <v>0.2545833333333333</v>
       </c>
       <c r="AR21">
-        <v>0.4564583333333333</v>
+        <v>0.2647916666666666</v>
       </c>
       <c r="AS21">
-        <v>0.475</v>
+        <v>0.275</v>
       </c>
     </row>
     <row r="22" spans="1:45">
@@ -33821,76 +34696,76 @@
         <v>0.03</v>
       </c>
       <c r="V22">
-        <v>0.04854166666666666</v>
+        <v>0.04020833333333333</v>
       </c>
       <c r="W22">
-        <v>0.06708333333333333</v>
+        <v>0.05041666666666667</v>
       </c>
       <c r="X22">
-        <v>0.08562499999999999</v>
+        <v>0.060625</v>
       </c>
       <c r="Y22">
-        <v>0.1041666666666667</v>
+        <v>0.07083333333333333</v>
       </c>
       <c r="Z22">
-        <v>0.1227083333333333</v>
+        <v>0.08104166666666666</v>
       </c>
       <c r="AA22">
-        <v>0.14125</v>
+        <v>0.09125</v>
       </c>
       <c r="AB22">
-        <v>0.1597916666666667</v>
+        <v>0.1014583333333333</v>
       </c>
       <c r="AC22">
-        <v>0.1783333333333333</v>
+        <v>0.1116666666666667</v>
       </c>
       <c r="AD22">
-        <v>0.196875</v>
+        <v>0.121875</v>
       </c>
       <c r="AE22">
-        <v>0.2154166666666666</v>
+        <v>0.1320833333333333</v>
       </c>
       <c r="AF22">
-        <v>0.2339583333333333</v>
+        <v>0.1422916666666666</v>
       </c>
       <c r="AG22">
-        <v>0.2525</v>
+        <v>0.1525</v>
       </c>
       <c r="AH22">
-        <v>0.2710416666666666</v>
+        <v>0.1627083333333333</v>
       </c>
       <c r="AI22">
-        <v>0.2895833333333334</v>
+        <v>0.1729166666666667</v>
       </c>
       <c r="AJ22">
-        <v>0.308125</v>
+        <v>0.183125</v>
       </c>
       <c r="AK22">
-        <v>0.3266666666666667</v>
+        <v>0.1933333333333334</v>
       </c>
       <c r="AL22">
-        <v>0.3452083333333333</v>
+        <v>0.2035416666666667</v>
       </c>
       <c r="AM22">
-        <v>0.36375</v>
+        <v>0.21375</v>
       </c>
       <c r="AN22">
-        <v>0.3822916666666666</v>
+        <v>0.2239583333333333</v>
       </c>
       <c r="AO22">
-        <v>0.4008333333333333</v>
+        <v>0.2341666666666667</v>
       </c>
       <c r="AP22">
-        <v>0.4193749999999999</v>
+        <v>0.244375</v>
       </c>
       <c r="AQ22">
-        <v>0.4379166666666666</v>
+        <v>0.2545833333333333</v>
       </c>
       <c r="AR22">
-        <v>0.4564583333333333</v>
+        <v>0.2647916666666666</v>
       </c>
       <c r="AS22">
-        <v>0.475</v>
+        <v>0.275</v>
       </c>
     </row>
     <row r="23" spans="1:45">
@@ -33946,76 +34821,76 @@
         <v>0.03</v>
       </c>
       <c r="V23">
-        <v>0.04854166666666666</v>
+        <v>0.04020833333333333</v>
       </c>
       <c r="W23">
-        <v>0.06708333333333333</v>
+        <v>0.05041666666666667</v>
       </c>
       <c r="X23">
-        <v>0.08562499999999999</v>
+        <v>0.060625</v>
       </c>
       <c r="Y23">
-        <v>0.1041666666666667</v>
+        <v>0.07083333333333333</v>
       </c>
       <c r="Z23">
-        <v>0.1227083333333333</v>
+        <v>0.08104166666666666</v>
       </c>
       <c r="AA23">
-        <v>0.14125</v>
+        <v>0.09125</v>
       </c>
       <c r="AB23">
-        <v>0.1597916666666667</v>
+        <v>0.1014583333333333</v>
       </c>
       <c r="AC23">
-        <v>0.1783333333333333</v>
+        <v>0.1116666666666667</v>
       </c>
       <c r="AD23">
-        <v>0.196875</v>
+        <v>0.121875</v>
       </c>
       <c r="AE23">
-        <v>0.2154166666666666</v>
+        <v>0.1320833333333333</v>
       </c>
       <c r="AF23">
-        <v>0.2339583333333333</v>
+        <v>0.1422916666666666</v>
       </c>
       <c r="AG23">
-        <v>0.2525</v>
+        <v>0.1525</v>
       </c>
       <c r="AH23">
-        <v>0.2710416666666666</v>
+        <v>0.1627083333333333</v>
       </c>
       <c r="AI23">
-        <v>0.2895833333333334</v>
+        <v>0.1729166666666667</v>
       </c>
       <c r="AJ23">
-        <v>0.308125</v>
+        <v>0.183125</v>
       </c>
       <c r="AK23">
-        <v>0.3266666666666667</v>
+        <v>0.1933333333333334</v>
       </c>
       <c r="AL23">
-        <v>0.3452083333333333</v>
+        <v>0.2035416666666667</v>
       </c>
       <c r="AM23">
-        <v>0.36375</v>
+        <v>0.21375</v>
       </c>
       <c r="AN23">
-        <v>0.3822916666666666</v>
+        <v>0.2239583333333333</v>
       </c>
       <c r="AO23">
-        <v>0.4008333333333333</v>
+        <v>0.2341666666666667</v>
       </c>
       <c r="AP23">
-        <v>0.4193749999999999</v>
+        <v>0.244375</v>
       </c>
       <c r="AQ23">
-        <v>0.4379166666666666</v>
+        <v>0.2545833333333333</v>
       </c>
       <c r="AR23">
-        <v>0.4564583333333333</v>
+        <v>0.2647916666666666</v>
       </c>
       <c r="AS23">
-        <v>0.475</v>
+        <v>0.275</v>
       </c>
     </row>
     <row r="24" spans="1:45">
@@ -34071,76 +34946,76 @@
         <v>0.0431010761323323</v>
       </c>
       <c r="V24">
-        <v>0.07672186462681846</v>
+        <v>0.06213853129348512</v>
       </c>
       <c r="W24">
-        <v>0.1103426531213046</v>
+        <v>0.08117598645463794</v>
       </c>
       <c r="X24">
-        <v>0.1439634416157908</v>
+        <v>0.1002134416157908</v>
       </c>
       <c r="Y24">
-        <v>0.1775842301102769</v>
+        <v>0.1192508967769436</v>
       </c>
       <c r="Z24">
-        <v>0.2112050186047631</v>
+        <v>0.1382883519380964</v>
       </c>
       <c r="AA24">
-        <v>0.2448258070992492</v>
+        <v>0.1573258070992492</v>
       </c>
       <c r="AB24">
-        <v>0.2784465955937354</v>
+        <v>0.1763632622604021</v>
       </c>
       <c r="AC24">
-        <v>0.3120673840882215</v>
+        <v>0.1954007174215548</v>
       </c>
       <c r="AD24">
-        <v>0.3456881725827077</v>
+        <v>0.2144381725827077</v>
       </c>
       <c r="AE24">
-        <v>0.3793089610771939</v>
+        <v>0.2334756277438605</v>
       </c>
       <c r="AF24">
-        <v>0.4129297495716799</v>
+        <v>0.2525130829050133</v>
       </c>
       <c r="AG24">
-        <v>0.4465505380661661</v>
+        <v>0.2715505380661661</v>
       </c>
       <c r="AH24">
-        <v>0.4801713265606523</v>
+        <v>0.2905879932273189</v>
       </c>
       <c r="AI24">
-        <v>0.5137921150551384</v>
+        <v>0.3096254483884718</v>
       </c>
       <c r="AJ24">
-        <v>0.5474129035496246</v>
+        <v>0.3286629035496246</v>
       </c>
       <c r="AK24">
-        <v>0.5810336920441107</v>
+        <v>0.3477003587107774</v>
       </c>
       <c r="AL24">
-        <v>0.6146544805385968</v>
+        <v>0.3667378138719303</v>
       </c>
       <c r="AM24">
-        <v>0.6482752690330831</v>
+        <v>0.3857752690330831</v>
       </c>
       <c r="AN24">
-        <v>0.6818960575275692</v>
+        <v>0.4048127241942359</v>
       </c>
       <c r="AO24">
-        <v>0.7155168460220555</v>
+        <v>0.4238501793553887</v>
       </c>
       <c r="AP24">
-        <v>0.7491376345165416</v>
+        <v>0.4428876345165416</v>
       </c>
       <c r="AQ24">
-        <v>0.7827584230110276</v>
+        <v>0.4619250896776944</v>
       </c>
       <c r="AR24">
-        <v>0.8163792115055138</v>
+        <v>0.4809625448388472</v>
       </c>
       <c r="AS24">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:45">
@@ -34321,76 +35196,76 @@
         <v>0.5</v>
       </c>
       <c r="V26">
-        <v>0.5145833333333334</v>
+        <v>0.5041666666666667</v>
       </c>
       <c r="W26">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="X26">
+        <v>0.5125</v>
+      </c>
+      <c r="Y26">
+        <v>0.5166666666666667</v>
+      </c>
+      <c r="Z26">
+        <v>0.5208333333333333</v>
+      </c>
+      <c r="AA26">
+        <v>0.525</v>
+      </c>
+      <c r="AB26">
         <v>0.5291666666666667</v>
       </c>
-      <c r="X26">
-        <v>0.54375</v>
-      </c>
-      <c r="Y26">
+      <c r="AC26">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AD26">
+        <v>0.5375</v>
+      </c>
+      <c r="AE26">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="AF26">
+        <v>0.5458333333333334</v>
+      </c>
+      <c r="AG26">
+        <v>0.55</v>
+      </c>
+      <c r="AH26">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="AI26">
         <v>0.5583333333333333</v>
       </c>
-      <c r="Z26">
-        <v>0.5729166666666666</v>
-      </c>
-      <c r="AA26">
+      <c r="AJ26">
+        <v>0.5625</v>
+      </c>
+      <c r="AK26">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="AL26">
+        <v>0.5708333333333333</v>
+      </c>
+      <c r="AM26">
+        <v>0.575</v>
+      </c>
+      <c r="AN26">
+        <v>0.5791666666666666</v>
+      </c>
+      <c r="AO26">
+        <v>0.5833333333333333</v>
+      </c>
+      <c r="AP26">
         <v>0.5875</v>
       </c>
-      <c r="AB26">
-        <v>0.6020833333333333</v>
-      </c>
-      <c r="AC26">
-        <v>0.6166666666666667</v>
-      </c>
-      <c r="AD26">
-        <v>0.63125</v>
-      </c>
-      <c r="AE26">
-        <v>0.6458333333333333</v>
-      </c>
-      <c r="AF26">
-        <v>0.6604166666666667</v>
-      </c>
-      <c r="AG26">
-        <v>0.675</v>
-      </c>
-      <c r="AH26">
-        <v>0.6895833333333333</v>
-      </c>
-      <c r="AI26">
-        <v>0.7041666666666666</v>
-      </c>
-      <c r="AJ26">
-        <v>0.71875</v>
-      </c>
-      <c r="AK26">
-        <v>0.7333333333333334</v>
-      </c>
-      <c r="AL26">
-        <v>0.7479166666666666</v>
-      </c>
-      <c r="AM26">
-        <v>0.7625</v>
-      </c>
-      <c r="AN26">
-        <v>0.7770833333333333</v>
-      </c>
-      <c r="AO26">
-        <v>0.7916666666666667</v>
-      </c>
-      <c r="AP26">
-        <v>0.80625</v>
-      </c>
       <c r="AQ26">
-        <v>0.8208333333333333</v>
+        <v>0.5916666666666666</v>
       </c>
       <c r="AR26">
-        <v>0.8354166666666667</v>
+        <v>0.5958333333333332</v>
       </c>
       <c r="AS26">
-        <v>0.85</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="27" spans="1:45">
@@ -34446,76 +35321,76 @@
         <v>0.0431010761323323</v>
       </c>
       <c r="V27">
-        <v>0.07672186462681846</v>
+        <v>0.06213853129348512</v>
       </c>
       <c r="W27">
-        <v>0.1103426531213046</v>
+        <v>0.08117598645463794</v>
       </c>
       <c r="X27">
-        <v>0.1439634416157908</v>
+        <v>0.1002134416157908</v>
       </c>
       <c r="Y27">
-        <v>0.1775842301102769</v>
+        <v>0.1192508967769436</v>
       </c>
       <c r="Z27">
-        <v>0.2112050186047631</v>
+        <v>0.1382883519380964</v>
       </c>
       <c r="AA27">
-        <v>0.2448258070992492</v>
+        <v>0.1573258070992492</v>
       </c>
       <c r="AB27">
-        <v>0.2784465955937354</v>
+        <v>0.1763632622604021</v>
       </c>
       <c r="AC27">
-        <v>0.3120673840882215</v>
+        <v>0.1954007174215548</v>
       </c>
       <c r="AD27">
-        <v>0.3456881725827077</v>
+        <v>0.2144381725827077</v>
       </c>
       <c r="AE27">
-        <v>0.3793089610771939</v>
+        <v>0.2334756277438605</v>
       </c>
       <c r="AF27">
-        <v>0.4129297495716799</v>
+        <v>0.2525130829050133</v>
       </c>
       <c r="AG27">
-        <v>0.4465505380661661</v>
+        <v>0.2715505380661661</v>
       </c>
       <c r="AH27">
-        <v>0.4801713265606523</v>
+        <v>0.2905879932273189</v>
       </c>
       <c r="AI27">
-        <v>0.5137921150551384</v>
+        <v>0.3096254483884718</v>
       </c>
       <c r="AJ27">
-        <v>0.5474129035496246</v>
+        <v>0.3286629035496246</v>
       </c>
       <c r="AK27">
-        <v>0.5810336920441107</v>
+        <v>0.3477003587107774</v>
       </c>
       <c r="AL27">
-        <v>0.6146544805385968</v>
+        <v>0.3667378138719303</v>
       </c>
       <c r="AM27">
-        <v>0.6482752690330831</v>
+        <v>0.3857752690330831</v>
       </c>
       <c r="AN27">
-        <v>0.6818960575275692</v>
+        <v>0.4048127241942359</v>
       </c>
       <c r="AO27">
-        <v>0.7155168460220555</v>
+        <v>0.4238501793553887</v>
       </c>
       <c r="AP27">
-        <v>0.7491376345165416</v>
+        <v>0.4428876345165416</v>
       </c>
       <c r="AQ27">
-        <v>0.7827584230110276</v>
+        <v>0.4619250896776944</v>
       </c>
       <c r="AR27">
-        <v>0.8163792115055138</v>
+        <v>0.4809625448388472</v>
       </c>
       <c r="AS27">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:45">
@@ -34571,76 +35446,76 @@
         <v>0.121359223300971</v>
       </c>
       <c r="V28">
-        <v>0.1577669902912623</v>
+        <v>0.1517192556634305</v>
       </c>
       <c r="W28">
-        <v>0.1941747572815535</v>
+        <v>0.1820792880258901</v>
       </c>
       <c r="X28">
-        <v>0.2305825242718448</v>
+        <v>0.2124393203883496</v>
       </c>
       <c r="Y28">
-        <v>0.266990291262136</v>
+        <v>0.2427993527508092</v>
       </c>
       <c r="Z28">
-        <v>0.3033980582524273</v>
+        <v>0.2731593851132687</v>
       </c>
       <c r="AA28">
-        <v>0.3398058252427185</v>
+        <v>0.3035194174757282</v>
       </c>
       <c r="AB28">
-        <v>0.3762135922330098</v>
+        <v>0.3338794498381878</v>
       </c>
       <c r="AC28">
-        <v>0.412621359223301</v>
+        <v>0.3642394822006473</v>
       </c>
       <c r="AD28">
-        <v>0.4490291262135923</v>
+        <v>0.3945995145631068</v>
       </c>
       <c r="AE28">
-        <v>0.4854368932038835</v>
+        <v>0.4249595469255664</v>
       </c>
       <c r="AF28">
-        <v>0.5218446601941747</v>
+        <v>0.4553195792880259</v>
       </c>
       <c r="AG28">
-        <v>0.558252427184466</v>
+        <v>0.4856796116504855</v>
       </c>
       <c r="AH28">
-        <v>0.5946601941747572</v>
+        <v>0.516039644012945</v>
       </c>
       <c r="AI28">
-        <v>0.6310679611650485</v>
+        <v>0.5463996763754047</v>
       </c>
       <c r="AJ28">
-        <v>0.6674757281553397</v>
+        <v>0.5767597087378641</v>
       </c>
       <c r="AK28">
-        <v>0.703883495145631</v>
+        <v>0.6071197411003236</v>
       </c>
       <c r="AL28">
-        <v>0.7402912621359223</v>
+        <v>0.6374797734627832</v>
       </c>
       <c r="AM28">
-        <v>0.7766990291262136</v>
+        <v>0.6678398058252427</v>
       </c>
       <c r="AN28">
-        <v>0.8131067961165048</v>
+        <v>0.6981998381877023</v>
       </c>
       <c r="AO28">
-        <v>0.8495145631067961</v>
+        <v>0.7285598705501619</v>
       </c>
       <c r="AP28">
-        <v>0.8859223300970872</v>
+        <v>0.7589199029126213</v>
       </c>
       <c r="AQ28">
-        <v>0.9223300970873785</v>
+        <v>0.7892799352750808</v>
       </c>
       <c r="AR28">
-        <v>0.9587378640776698</v>
+        <v>0.8196399676375404</v>
       </c>
       <c r="AS28">
-        <v>0.9951456310679611</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="29" spans="1:45">
@@ -34696,76 +35571,76 @@
         <v>0.87378640776699</v>
       </c>
       <c r="V29">
-        <v>0.8373786407766988</v>
+        <v>0.8434263754045305</v>
       </c>
       <c r="W29">
-        <v>0.8009708737864075</v>
+        <v>0.8130663430420709</v>
       </c>
       <c r="X29">
-        <v>0.7645631067961163</v>
+        <v>0.7827063106796114</v>
       </c>
       <c r="Y29">
-        <v>0.728155339805825</v>
+        <v>0.7523462783171518</v>
       </c>
       <c r="Z29">
-        <v>0.6917475728155338</v>
+        <v>0.7219862459546923</v>
       </c>
       <c r="AA29">
-        <v>0.6553398058252425</v>
+        <v>0.6916262135922329</v>
       </c>
       <c r="AB29">
-        <v>0.6189320388349512</v>
+        <v>0.6612661812297732</v>
       </c>
       <c r="AC29">
-        <v>0.58252427184466</v>
+        <v>0.6309061488673138</v>
       </c>
       <c r="AD29">
-        <v>0.5461165048543688</v>
+        <v>0.6005461165048542</v>
       </c>
       <c r="AE29">
-        <v>0.5097087378640774</v>
+        <v>0.5701860841423946</v>
       </c>
       <c r="AF29">
-        <v>0.4733009708737863</v>
+        <v>0.5398260517799351</v>
       </c>
       <c r="AG29">
-        <v>0.436893203883495</v>
+        <v>0.5094660194174756</v>
       </c>
       <c r="AH29">
-        <v>0.4004854368932038</v>
+        <v>0.479105987055016</v>
       </c>
       <c r="AI29">
-        <v>0.3640776699029125</v>
+        <v>0.4487459546925564</v>
       </c>
       <c r="AJ29">
-        <v>0.3276699029126213</v>
+        <v>0.418385922330097</v>
       </c>
       <c r="AK29">
-        <v>0.29126213592233</v>
+        <v>0.3880258899676374</v>
       </c>
       <c r="AL29">
-        <v>0.2548543689320387</v>
+        <v>0.3576658576051778</v>
       </c>
       <c r="AM29">
-        <v>0.2184466019417475</v>
+        <v>0.3273058252427183</v>
       </c>
       <c r="AN29">
-        <v>0.1820388349514563</v>
+        <v>0.2969457928802588</v>
       </c>
       <c r="AO29">
-        <v>0.145631067961165</v>
+        <v>0.2665857605177993</v>
       </c>
       <c r="AP29">
-        <v>0.1092233009708738</v>
+        <v>0.2362257281553397</v>
       </c>
       <c r="AQ29">
-        <v>0.07281553398058253</v>
+        <v>0.2058656957928802</v>
       </c>
       <c r="AR29">
-        <v>0.03640776699029122</v>
+        <v>0.1755056634304206</v>
       </c>
       <c r="AS29">
-        <v>0</v>
+        <v>0.1451456310679611</v>
       </c>
     </row>
     <row r="30" spans="1:45">
@@ -34821,76 +35696,76 @@
         <v>0.05</v>
       </c>
       <c r="V30">
+        <v>0.06875000000000001</v>
+      </c>
+      <c r="W30">
         <v>0.08749999999999999</v>
       </c>
-      <c r="W30">
+      <c r="X30">
+        <v>0.10625</v>
+      </c>
+      <c r="Y30">
         <v>0.125</v>
       </c>
-      <c r="X30">
+      <c r="Z30">
+        <v>0.14375</v>
+      </c>
+      <c r="AA30">
         <v>0.1625</v>
       </c>
-      <c r="Y30">
+      <c r="AB30">
+        <v>0.18125</v>
+      </c>
+      <c r="AC30">
         <v>0.2</v>
       </c>
-      <c r="Z30">
+      <c r="AD30">
+        <v>0.21875</v>
+      </c>
+      <c r="AE30">
         <v>0.2375</v>
       </c>
-      <c r="AA30">
+      <c r="AF30">
+        <v>0.25625</v>
+      </c>
+      <c r="AG30">
         <v>0.275</v>
       </c>
-      <c r="AB30">
+      <c r="AH30">
+        <v>0.29375</v>
+      </c>
+      <c r="AI30">
         <v>0.3125</v>
       </c>
-      <c r="AC30">
+      <c r="AJ30">
+        <v>0.33125</v>
+      </c>
+      <c r="AK30">
         <v>0.35</v>
       </c>
-      <c r="AD30">
+      <c r="AL30">
+        <v>0.36875</v>
+      </c>
+      <c r="AM30">
         <v>0.3875</v>
       </c>
-      <c r="AE30">
+      <c r="AN30">
+        <v>0.40625</v>
+      </c>
+      <c r="AO30">
         <v>0.425</v>
       </c>
-      <c r="AF30">
+      <c r="AP30">
+        <v>0.44375</v>
+      </c>
+      <c r="AQ30">
         <v>0.4625</v>
       </c>
-      <c r="AG30">
+      <c r="AR30">
+        <v>0.48125</v>
+      </c>
+      <c r="AS30">
         <v>0.5</v>
-      </c>
-      <c r="AH30">
-        <v>0.5375</v>
-      </c>
-      <c r="AI30">
-        <v>0.5750000000000001</v>
-      </c>
-      <c r="AJ30">
-        <v>0.6125</v>
-      </c>
-      <c r="AK30">
-        <v>0.65</v>
-      </c>
-      <c r="AL30">
-        <v>0.6875</v>
-      </c>
-      <c r="AM30">
-        <v>0.7249999999999999</v>
-      </c>
-      <c r="AN30">
-        <v>0.7624999999999998</v>
-      </c>
-      <c r="AO30">
-        <v>0.7999999999999999</v>
-      </c>
-      <c r="AP30">
-        <v>0.8374999999999999</v>
-      </c>
-      <c r="AQ30">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="AR30">
-        <v>0.9125</v>
-      </c>
-      <c r="AS30">
-        <v>0.95</v>
       </c>
     </row>
     <row r="31" spans="1:45">
@@ -34946,76 +35821,76 @@
         <v>0.05</v>
       </c>
       <c r="V31">
+        <v>0.06875000000000001</v>
+      </c>
+      <c r="W31">
         <v>0.08749999999999999</v>
       </c>
-      <c r="W31">
+      <c r="X31">
+        <v>0.10625</v>
+      </c>
+      <c r="Y31">
         <v>0.125</v>
       </c>
-      <c r="X31">
+      <c r="Z31">
+        <v>0.14375</v>
+      </c>
+      <c r="AA31">
         <v>0.1625</v>
       </c>
-      <c r="Y31">
+      <c r="AB31">
+        <v>0.18125</v>
+      </c>
+      <c r="AC31">
         <v>0.2</v>
       </c>
-      <c r="Z31">
+      <c r="AD31">
+        <v>0.21875</v>
+      </c>
+      <c r="AE31">
         <v>0.2375</v>
       </c>
-      <c r="AA31">
+      <c r="AF31">
+        <v>0.25625</v>
+      </c>
+      <c r="AG31">
         <v>0.275</v>
       </c>
-      <c r="AB31">
+      <c r="AH31">
+        <v>0.29375</v>
+      </c>
+      <c r="AI31">
         <v>0.3125</v>
       </c>
-      <c r="AC31">
+      <c r="AJ31">
+        <v>0.33125</v>
+      </c>
+      <c r="AK31">
         <v>0.35</v>
       </c>
-      <c r="AD31">
+      <c r="AL31">
+        <v>0.36875</v>
+      </c>
+      <c r="AM31">
         <v>0.3875</v>
       </c>
-      <c r="AE31">
+      <c r="AN31">
+        <v>0.40625</v>
+      </c>
+      <c r="AO31">
         <v>0.425</v>
       </c>
-      <c r="AF31">
+      <c r="AP31">
+        <v>0.44375</v>
+      </c>
+      <c r="AQ31">
         <v>0.4625</v>
       </c>
-      <c r="AG31">
+      <c r="AR31">
+        <v>0.48125</v>
+      </c>
+      <c r="AS31">
         <v>0.5</v>
-      </c>
-      <c r="AH31">
-        <v>0.5375</v>
-      </c>
-      <c r="AI31">
-        <v>0.5750000000000001</v>
-      </c>
-      <c r="AJ31">
-        <v>0.6125</v>
-      </c>
-      <c r="AK31">
-        <v>0.65</v>
-      </c>
-      <c r="AL31">
-        <v>0.6875</v>
-      </c>
-      <c r="AM31">
-        <v>0.7249999999999999</v>
-      </c>
-      <c r="AN31">
-        <v>0.7624999999999998</v>
-      </c>
-      <c r="AO31">
-        <v>0.7999999999999999</v>
-      </c>
-      <c r="AP31">
-        <v>0.8374999999999999</v>
-      </c>
-      <c r="AQ31">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="AR31">
-        <v>0.9125</v>
-      </c>
-      <c r="AS31">
-        <v>0.95</v>
       </c>
     </row>
     <row r="32" spans="1:45">
@@ -35071,76 +35946,76 @@
         <v>0.05</v>
       </c>
       <c r="V32">
+        <v>0.06875000000000001</v>
+      </c>
+      <c r="W32">
         <v>0.08749999999999999</v>
       </c>
-      <c r="W32">
+      <c r="X32">
+        <v>0.10625</v>
+      </c>
+      <c r="Y32">
         <v>0.125</v>
       </c>
-      <c r="X32">
+      <c r="Z32">
+        <v>0.14375</v>
+      </c>
+      <c r="AA32">
         <v>0.1625</v>
       </c>
-      <c r="Y32">
+      <c r="AB32">
+        <v>0.18125</v>
+      </c>
+      <c r="AC32">
         <v>0.2</v>
       </c>
-      <c r="Z32">
+      <c r="AD32">
+        <v>0.21875</v>
+      </c>
+      <c r="AE32">
         <v>0.2375</v>
       </c>
-      <c r="AA32">
+      <c r="AF32">
+        <v>0.25625</v>
+      </c>
+      <c r="AG32">
         <v>0.275</v>
       </c>
-      <c r="AB32">
+      <c r="AH32">
+        <v>0.29375</v>
+      </c>
+      <c r="AI32">
         <v>0.3125</v>
       </c>
-      <c r="AC32">
+      <c r="AJ32">
+        <v>0.33125</v>
+      </c>
+      <c r="AK32">
         <v>0.35</v>
       </c>
-      <c r="AD32">
+      <c r="AL32">
+        <v>0.36875</v>
+      </c>
+      <c r="AM32">
         <v>0.3875</v>
       </c>
-      <c r="AE32">
+      <c r="AN32">
+        <v>0.40625</v>
+      </c>
+      <c r="AO32">
         <v>0.425</v>
       </c>
-      <c r="AF32">
+      <c r="AP32">
+        <v>0.44375</v>
+      </c>
+      <c r="AQ32">
         <v>0.4625</v>
       </c>
-      <c r="AG32">
+      <c r="AR32">
+        <v>0.48125</v>
+      </c>
+      <c r="AS32">
         <v>0.5</v>
-      </c>
-      <c r="AH32">
-        <v>0.5375</v>
-      </c>
-      <c r="AI32">
-        <v>0.5750000000000001</v>
-      </c>
-      <c r="AJ32">
-        <v>0.6125</v>
-      </c>
-      <c r="AK32">
-        <v>0.65</v>
-      </c>
-      <c r="AL32">
-        <v>0.6875</v>
-      </c>
-      <c r="AM32">
-        <v>0.7249999999999999</v>
-      </c>
-      <c r="AN32">
-        <v>0.7624999999999998</v>
-      </c>
-      <c r="AO32">
-        <v>0.7999999999999999</v>
-      </c>
-      <c r="AP32">
-        <v>0.8374999999999999</v>
-      </c>
-      <c r="AQ32">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="AR32">
-        <v>0.9125</v>
-      </c>
-      <c r="AS32">
-        <v>0.95</v>
       </c>
     </row>
     <row r="33" spans="1:45">
@@ -35196,76 +36071,76 @@
         <v>0.05</v>
       </c>
       <c r="V33">
+        <v>0.06875000000000001</v>
+      </c>
+      <c r="W33">
         <v>0.08749999999999999</v>
       </c>
-      <c r="W33">
+      <c r="X33">
+        <v>0.10625</v>
+      </c>
+      <c r="Y33">
         <v>0.125</v>
       </c>
-      <c r="X33">
+      <c r="Z33">
+        <v>0.14375</v>
+      </c>
+      <c r="AA33">
         <v>0.1625</v>
       </c>
-      <c r="Y33">
+      <c r="AB33">
+        <v>0.18125</v>
+      </c>
+      <c r="AC33">
         <v>0.2</v>
       </c>
-      <c r="Z33">
+      <c r="AD33">
+        <v>0.21875</v>
+      </c>
+      <c r="AE33">
         <v>0.2375</v>
       </c>
-      <c r="AA33">
+      <c r="AF33">
+        <v>0.25625</v>
+      </c>
+      <c r="AG33">
         <v>0.275</v>
       </c>
-      <c r="AB33">
+      <c r="AH33">
+        <v>0.29375</v>
+      </c>
+      <c r="AI33">
         <v>0.3125</v>
       </c>
-      <c r="AC33">
+      <c r="AJ33">
+        <v>0.33125</v>
+      </c>
+      <c r="AK33">
         <v>0.35</v>
       </c>
-      <c r="AD33">
+      <c r="AL33">
+        <v>0.36875</v>
+      </c>
+      <c r="AM33">
         <v>0.3875</v>
       </c>
-      <c r="AE33">
+      <c r="AN33">
+        <v>0.40625</v>
+      </c>
+      <c r="AO33">
         <v>0.425</v>
       </c>
-      <c r="AF33">
+      <c r="AP33">
+        <v>0.44375</v>
+      </c>
+      <c r="AQ33">
         <v>0.4625</v>
       </c>
-      <c r="AG33">
+      <c r="AR33">
+        <v>0.48125</v>
+      </c>
+      <c r="AS33">
         <v>0.5</v>
-      </c>
-      <c r="AH33">
-        <v>0.5375</v>
-      </c>
-      <c r="AI33">
-        <v>0.5750000000000001</v>
-      </c>
-      <c r="AJ33">
-        <v>0.6125</v>
-      </c>
-      <c r="AK33">
-        <v>0.65</v>
-      </c>
-      <c r="AL33">
-        <v>0.6875</v>
-      </c>
-      <c r="AM33">
-        <v>0.7249999999999999</v>
-      </c>
-      <c r="AN33">
-        <v>0.7624999999999998</v>
-      </c>
-      <c r="AO33">
-        <v>0.7999999999999999</v>
-      </c>
-      <c r="AP33">
-        <v>0.8374999999999999</v>
-      </c>
-      <c r="AQ33">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="AR33">
-        <v>0.9125</v>
-      </c>
-      <c r="AS33">
-        <v>0.95</v>
       </c>
     </row>
     <row r="34" spans="1:45">
@@ -35321,76 +36196,76 @@
         <v>0.05</v>
       </c>
       <c r="V34">
+        <v>0.06875000000000001</v>
+      </c>
+      <c r="W34">
         <v>0.08749999999999999</v>
       </c>
-      <c r="W34">
+      <c r="X34">
+        <v>0.10625</v>
+      </c>
+      <c r="Y34">
         <v>0.125</v>
       </c>
-      <c r="X34">
+      <c r="Z34">
+        <v>0.14375</v>
+      </c>
+      <c r="AA34">
         <v>0.1625</v>
       </c>
-      <c r="Y34">
+      <c r="AB34">
+        <v>0.18125</v>
+      </c>
+      <c r="AC34">
         <v>0.2</v>
       </c>
-      <c r="Z34">
+      <c r="AD34">
+        <v>0.21875</v>
+      </c>
+      <c r="AE34">
         <v>0.2375</v>
       </c>
-      <c r="AA34">
+      <c r="AF34">
+        <v>0.25625</v>
+      </c>
+      <c r="AG34">
         <v>0.275</v>
       </c>
-      <c r="AB34">
+      <c r="AH34">
+        <v>0.29375</v>
+      </c>
+      <c r="AI34">
         <v>0.3125</v>
       </c>
-      <c r="AC34">
+      <c r="AJ34">
+        <v>0.33125</v>
+      </c>
+      <c r="AK34">
         <v>0.35</v>
       </c>
-      <c r="AD34">
+      <c r="AL34">
+        <v>0.36875</v>
+      </c>
+      <c r="AM34">
         <v>0.3875</v>
       </c>
-      <c r="AE34">
+      <c r="AN34">
+        <v>0.40625</v>
+      </c>
+      <c r="AO34">
         <v>0.425</v>
       </c>
-      <c r="AF34">
+      <c r="AP34">
+        <v>0.44375</v>
+      </c>
+      <c r="AQ34">
         <v>0.4625</v>
       </c>
-      <c r="AG34">
+      <c r="AR34">
+        <v>0.48125</v>
+      </c>
+      <c r="AS34">
         <v>0.5</v>
-      </c>
-      <c r="AH34">
-        <v>0.5375</v>
-      </c>
-      <c r="AI34">
-        <v>0.5750000000000001</v>
-      </c>
-      <c r="AJ34">
-        <v>0.6125</v>
-      </c>
-      <c r="AK34">
-        <v>0.65</v>
-      </c>
-      <c r="AL34">
-        <v>0.6875</v>
-      </c>
-      <c r="AM34">
-        <v>0.7249999999999999</v>
-      </c>
-      <c r="AN34">
-        <v>0.7624999999999998</v>
-      </c>
-      <c r="AO34">
-        <v>0.7999999999999999</v>
-      </c>
-      <c r="AP34">
-        <v>0.8374999999999999</v>
-      </c>
-      <c r="AQ34">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="AR34">
-        <v>0.9125</v>
-      </c>
-      <c r="AS34">
-        <v>0.95</v>
       </c>
     </row>
     <row r="35" spans="1:45">
@@ -35446,76 +36321,76 @@
         <v>0.05</v>
       </c>
       <c r="V35">
+        <v>0.06875000000000001</v>
+      </c>
+      <c r="W35">
         <v>0.08749999999999999</v>
       </c>
-      <c r="W35">
+      <c r="X35">
+        <v>0.10625</v>
+      </c>
+      <c r="Y35">
         <v>0.125</v>
       </c>
-      <c r="X35">
+      <c r="Z35">
+        <v>0.14375</v>
+      </c>
+      <c r="AA35">
         <v>0.1625</v>
       </c>
-      <c r="Y35">
+      <c r="AB35">
+        <v>0.18125</v>
+      </c>
+      <c r="AC35">
         <v>0.2</v>
       </c>
-      <c r="Z35">
+      <c r="AD35">
+        <v>0.21875</v>
+      </c>
+      <c r="AE35">
         <v>0.2375</v>
       </c>
-      <c r="AA35">
+      <c r="AF35">
+        <v>0.25625</v>
+      </c>
+      <c r="AG35">
         <v>0.275</v>
       </c>
-      <c r="AB35">
+      <c r="AH35">
+        <v>0.29375</v>
+      </c>
+      <c r="AI35">
         <v>0.3125</v>
       </c>
-      <c r="AC35">
+      <c r="AJ35">
+        <v>0.33125</v>
+      </c>
+      <c r="AK35">
         <v>0.35</v>
       </c>
-      <c r="AD35">
+      <c r="AL35">
+        <v>0.36875</v>
+      </c>
+      <c r="AM35">
         <v>0.3875</v>
       </c>
-      <c r="AE35">
+      <c r="AN35">
+        <v>0.40625</v>
+      </c>
+      <c r="AO35">
         <v>0.425</v>
       </c>
-      <c r="AF35">
+      <c r="AP35">
+        <v>0.44375</v>
+      </c>
+      <c r="AQ35">
         <v>0.4625</v>
       </c>
-      <c r="AG35">
+      <c r="AR35">
+        <v>0.48125</v>
+      </c>
+      <c r="AS35">
         <v>0.5</v>
-      </c>
-      <c r="AH35">
-        <v>0.5375</v>
-      </c>
-      <c r="AI35">
-        <v>0.5750000000000001</v>
-      </c>
-      <c r="AJ35">
-        <v>0.6125</v>
-      </c>
-      <c r="AK35">
-        <v>0.65</v>
-      </c>
-      <c r="AL35">
-        <v>0.6875</v>
-      </c>
-      <c r="AM35">
-        <v>0.7249999999999999</v>
-      </c>
-      <c r="AN35">
-        <v>0.7624999999999998</v>
-      </c>
-      <c r="AO35">
-        <v>0.7999999999999999</v>
-      </c>
-      <c r="AP35">
-        <v>0.8374999999999999</v>
-      </c>
-      <c r="AQ35">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="AR35">
-        <v>0.9125</v>
-      </c>
-      <c r="AS35">
-        <v>0.95</v>
       </c>
     </row>
     <row r="36" spans="1:45">
@@ -35571,76 +36446,76 @@
         <v>0.05</v>
       </c>
       <c r="V36">
+        <v>0.06875000000000001</v>
+      </c>
+      <c r="W36">
         <v>0.08749999999999999</v>
       </c>
-      <c r="W36">
+      <c r="X36">
+        <v>0.10625</v>
+      </c>
+      <c r="Y36">
         <v>0.125</v>
       </c>
-      <c r="X36">
+      <c r="Z36">
+        <v>0.14375</v>
+      </c>
+      <c r="AA36">
         <v>0.1625</v>
       </c>
-      <c r="Y36">
+      <c r="AB36">
+        <v>0.18125</v>
+      </c>
+      <c r="AC36">
         <v>0.2</v>
       </c>
-      <c r="Z36">
+      <c r="AD36">
+        <v>0.21875</v>
+      </c>
+      <c r="AE36">
         <v>0.2375</v>
       </c>
-      <c r="AA36">
+      <c r="AF36">
+        <v>0.25625</v>
+      </c>
+      <c r="AG36">
         <v>0.275</v>
       </c>
-      <c r="AB36">
+      <c r="AH36">
+        <v>0.29375</v>
+      </c>
+      <c r="AI36">
         <v>0.3125</v>
       </c>
-      <c r="AC36">
+      <c r="AJ36">
+        <v>0.33125</v>
+      </c>
+      <c r="AK36">
         <v>0.35</v>
       </c>
-      <c r="AD36">
+      <c r="AL36">
+        <v>0.36875</v>
+      </c>
+      <c r="AM36">
         <v>0.3875</v>
       </c>
-      <c r="AE36">
+      <c r="AN36">
+        <v>0.40625</v>
+      </c>
+      <c r="AO36">
         <v>0.425</v>
       </c>
-      <c r="AF36">
+      <c r="AP36">
+        <v>0.44375</v>
+      </c>
+      <c r="AQ36">
         <v>0.4625</v>
       </c>
-      <c r="AG36">
+      <c r="AR36">
+        <v>0.48125</v>
+      </c>
+      <c r="AS36">
         <v>0.5</v>
-      </c>
-      <c r="AH36">
-        <v>0.5375</v>
-      </c>
-      <c r="AI36">
-        <v>0.5750000000000001</v>
-      </c>
-      <c r="AJ36">
-        <v>0.6125</v>
-      </c>
-      <c r="AK36">
-        <v>0.65</v>
-      </c>
-      <c r="AL36">
-        <v>0.6875</v>
-      </c>
-      <c r="AM36">
-        <v>0.7249999999999999</v>
-      </c>
-      <c r="AN36">
-        <v>0.7624999999999998</v>
-      </c>
-      <c r="AO36">
-        <v>0.7999999999999999</v>
-      </c>
-      <c r="AP36">
-        <v>0.8374999999999999</v>
-      </c>
-      <c r="AQ36">
-        <v>0.8749999999999999</v>
-      </c>
-      <c r="AR36">
-        <v>0.9125</v>
-      </c>
-      <c r="AS36">
-        <v>0.95</v>
       </c>
     </row>
     <row r="37" spans="1:45">
@@ -38590,76 +39465,76 @@
         <v>1</v>
       </c>
       <c r="V18">
-        <v>0.9875</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="W18">
-        <v>0.975</v>
+        <v>0.95</v>
       </c>
       <c r="X18">
-        <v>0.9625</v>
+        <v>0.925</v>
       </c>
       <c r="Y18">
-        <v>0.9500000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="Z18">
-        <v>0.9375</v>
+        <v>0.875</v>
       </c>
       <c r="AA18">
-        <v>0.925</v>
+        <v>0.85</v>
       </c>
       <c r="AB18">
-        <v>0.9124999999999999</v>
+        <v>0.825</v>
       </c>
       <c r="AC18">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="AD18">
-        <v>0.8875</v>
+        <v>0.775</v>
       </c>
       <c r="AE18">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="AF18">
-        <v>0.8625</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="AG18">
-        <v>0.85</v>
+        <v>0.7</v>
       </c>
       <c r="AH18">
-        <v>0.8374999999999999</v>
+        <v>0.675</v>
       </c>
       <c r="AI18">
-        <v>0.825</v>
+        <v>0.65</v>
       </c>
       <c r="AJ18">
-        <v>0.8125</v>
+        <v>0.625</v>
       </c>
       <c r="AK18">
-        <v>0.8</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="AL18">
-        <v>0.7875</v>
+        <v>0.575</v>
       </c>
       <c r="AM18">
-        <v>0.7749999999999999</v>
+        <v>0.55</v>
       </c>
       <c r="AN18">
-        <v>0.7625</v>
+        <v>0.525</v>
       </c>
       <c r="AO18">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AP18">
-        <v>0.7374999999999999</v>
+        <v>0.475</v>
       </c>
       <c r="AQ18">
-        <v>0.725</v>
+        <v>0.4500000000000001</v>
       </c>
       <c r="AR18">
-        <v>0.7124999999999999</v>
+        <v>0.425</v>
       </c>
       <c r="AS18">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:45">

</xml_diff>